<commit_message>
same name projects resolved
</commit_message>
<xml_diff>
--- a/data/pool.xlsx
+++ b/data/pool.xlsx
@@ -25,10 +25,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -86,6 +88,9 @@
       <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="30">
@@ -264,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -405,6 +410,12 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -434,7 +445,7 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -1122,6 +1133,10 @@
     <xf numFmtId="0" fontId="5" fillId="29" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2114,1156 +2129,1816 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:BC20"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
-  <cols>
-    <col width="24.15" customWidth="1" style="105" min="1" max="1"/>
-    <col width="14.28" customWidth="1" style="105" min="2" max="2"/>
-    <col width="18.42" customWidth="1" style="105" min="3" max="3"/>
-    <col width="13.86" customWidth="1" style="105" min="4" max="4"/>
-    <col width="14.43" customWidth="1" style="105" min="5" max="5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="117.75" customHeight="1" s="106">
-      <c r="A1" s="107" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="211" t="inlineStr">
         <is>
           <t>Projects</t>
         </is>
       </c>
-      <c r="B1" s="108" t="inlineStr">
+      <c r="B1" s="211" t="inlineStr">
         <is>
           <t>Leading Institution</t>
         </is>
       </c>
-      <c r="C1" s="109" t="inlineStr">
+      <c r="C1" s="211" t="inlineStr">
         <is>
           <t>Partner institution(s)</t>
         </is>
       </c>
-      <c r="D1" s="110" t="inlineStr">
+      <c r="D1" s="211" t="inlineStr">
         <is>
           <t>pickup_date</t>
         </is>
       </c>
-      <c r="E1" s="111" t="inlineStr">
+      <c r="E1" s="211" t="inlineStr">
         <is>
           <t>return_date</t>
         </is>
       </c>
-      <c r="F1" s="112">
-        <f>'[1]FINNSIP inventory 2023'!$B2</f>
-        <v/>
-      </c>
-      <c r="G1" s="113">
-        <f>'[1]FINNSIP inventory 2023'!$B3</f>
-        <v/>
-      </c>
-      <c r="H1" s="114">
-        <f>'[1]FINNSIP inventory 2023'!$B4</f>
-        <v/>
-      </c>
-      <c r="I1" s="115">
-        <f>'[1]FINNSIP inventory 2023'!$B5</f>
-        <v/>
-      </c>
-      <c r="J1" s="116">
-        <f>'[1]FINNSIP inventory 2023'!$B6</f>
-        <v/>
-      </c>
-      <c r="K1" s="117">
-        <f>'[1]FINNSIP inventory 2023'!$B7</f>
-        <v/>
-      </c>
-      <c r="L1" s="118">
-        <f>'[1]FINNSIP inventory 2023'!$B8</f>
-        <v/>
-      </c>
-      <c r="M1" s="119">
-        <f>'[1]FINNSIP inventory 2023'!$B9</f>
-        <v/>
-      </c>
-      <c r="N1" s="120">
-        <f>'[1]FINNSIP inventory 2023'!$B10</f>
-        <v/>
-      </c>
-      <c r="O1" s="121">
-        <f>'[1]FINNSIP inventory 2023'!$B11</f>
-        <v/>
-      </c>
-      <c r="P1" s="122">
-        <f>'[1]FINNSIP inventory 2023'!$B12</f>
-        <v/>
-      </c>
-      <c r="Q1" s="123">
-        <f>'[1]FINNSIP inventory 2023'!$B13</f>
-        <v/>
-      </c>
-      <c r="R1" s="124">
-        <f>'[1]FINNSIP inventory 2023'!$B14</f>
-        <v/>
-      </c>
-      <c r="S1" s="125">
-        <f>'[1]FINNSIP inventory 2023'!$B15</f>
-        <v/>
-      </c>
-      <c r="T1" s="126">
-        <f>'[1]FINNSIP inventory 2023'!$B16</f>
-        <v/>
-      </c>
-      <c r="U1" s="127">
-        <f>'[1]FINNSIP inventory 2023'!$B17</f>
-        <v/>
-      </c>
-      <c r="V1" s="128">
-        <f>'[1]FINNSIP inventory 2023'!$B18</f>
-        <v/>
-      </c>
-      <c r="W1" s="129">
-        <f>'[1]FINNSIP inventory 2023'!$B19</f>
-        <v/>
-      </c>
-      <c r="X1" s="130">
-        <f>'[1]FINNSIP inventory 2023'!$B20</f>
-        <v/>
-      </c>
-      <c r="Y1" s="131">
-        <f>'[1]FINNSIP inventory 2023'!$B21</f>
-        <v/>
-      </c>
-      <c r="Z1" s="132">
-        <f>'[1]FINNSIP inventory 2023'!$B22</f>
-        <v/>
-      </c>
-      <c r="AA1" s="133">
-        <f>'[1]FINNSIP inventory 2023'!$B23</f>
-        <v/>
-      </c>
-      <c r="AB1" s="134">
-        <f>'[1]FINNSIP inventory 2023'!$B24</f>
-        <v/>
-      </c>
-      <c r="AC1" s="135">
-        <f>'[1]FINNSIP inventory 2023'!$B25</f>
-        <v/>
-      </c>
-      <c r="AD1" s="136">
-        <f>'[1]FINNSIP inventory 2023'!$B26</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="106">
-      <c r="A2" s="137" t="inlineStr">
+      <c r="F1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 10</t>
+        </is>
+      </c>
+      <c r="L1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 11</t>
+        </is>
+      </c>
+      <c r="M1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 13</t>
+        </is>
+      </c>
+      <c r="O1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 14</t>
+        </is>
+      </c>
+      <c r="P1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 15</t>
+        </is>
+      </c>
+      <c r="Q1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 16</t>
+        </is>
+      </c>
+      <c r="R1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 17</t>
+        </is>
+      </c>
+      <c r="S1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 18</t>
+        </is>
+      </c>
+      <c r="T1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 19</t>
+        </is>
+      </c>
+      <c r="U1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 20</t>
+        </is>
+      </c>
+      <c r="V1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 21</t>
+        </is>
+      </c>
+      <c r="W1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 22</t>
+        </is>
+      </c>
+      <c r="X1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 23</t>
+        </is>
+      </c>
+      <c r="Y1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 24</t>
+        </is>
+      </c>
+      <c r="Z1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 25</t>
+        </is>
+      </c>
+      <c r="AA1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 26</t>
+        </is>
+      </c>
+      <c r="AB1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 27</t>
+        </is>
+      </c>
+      <c r="AC1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 28</t>
+        </is>
+      </c>
+      <c r="AD1" s="211" t="inlineStr">
+        <is>
+          <t>Unnamed: 29</t>
+        </is>
+      </c>
+      <c r="AE1" s="211" t="inlineStr">
+        <is>
+          <t>GSB3</t>
+        </is>
+      </c>
+      <c r="AF1" s="211" t="inlineStr">
+        <is>
+          <t>GS-ONE5HZ</t>
+        </is>
+      </c>
+      <c r="AG1" s="211" t="inlineStr">
+        <is>
+          <t>GSX3</t>
+        </is>
+      </c>
+      <c r="AH1" s="211" t="inlineStr">
+        <is>
+          <t>LHR</t>
+        </is>
+      </c>
+      <c r="AI1" s="211" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="AJ1" s="211" t="inlineStr">
+        <is>
+          <t>BN25</t>
+        </is>
+      </c>
+      <c r="AK1" s="211" t="inlineStr">
+        <is>
+          <t>BN32</t>
+        </is>
+      </c>
+      <c r="AL1" s="211" t="inlineStr">
+        <is>
+          <t>DTM48</t>
+        </is>
+      </c>
+      <c r="AM1" s="211" t="inlineStr">
+        <is>
+          <t>DTM24</t>
+        </is>
+      </c>
+      <c r="AN1" s="211" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="AO1" s="211" t="inlineStr">
+        <is>
+          <t>BMS12</t>
+        </is>
+      </c>
+      <c r="AP1" s="211" t="inlineStr">
+        <is>
+          <t>TOUGHBOOK</t>
+        </is>
+      </c>
+      <c r="AQ1" s="211" t="inlineStr">
+        <is>
+          <t>ZBOOK</t>
+        </is>
+      </c>
+      <c r="AR1" s="211" t="inlineStr">
+        <is>
+          <t>IGU-16HR3C</t>
+        </is>
+      </c>
+      <c r="AS1" s="211" t="inlineStr">
+        <is>
+          <t>SmartsoloCharger</t>
+        </is>
+      </c>
+      <c r="AT1" s="211" t="inlineStr">
+        <is>
+          <t>SmartsoloRack</t>
+        </is>
+      </c>
+      <c r="AU1" s="211" t="inlineStr">
+        <is>
+          <t>MAGNET</t>
+        </is>
+      </c>
+      <c r="AV1" s="211" t="inlineStr">
+        <is>
+          <t>SDRX</t>
+        </is>
+      </c>
+      <c r="AW1" s="211" t="inlineStr">
+        <is>
+          <t>MINIMUS</t>
+        </is>
+      </c>
+      <c r="AX1" s="211" t="inlineStr">
+        <is>
+          <t>3ESPC</t>
+        </is>
+      </c>
+      <c r="AY1" s="211" t="inlineStr">
+        <is>
+          <t>GNSS</t>
+        </is>
+      </c>
+      <c r="AZ1" s="211" t="inlineStr">
+        <is>
+          <t>CABLEBB</t>
+        </is>
+      </c>
+      <c r="BA1" s="211" t="inlineStr">
+        <is>
+          <t>MASCOT</t>
+        </is>
+      </c>
+      <c r="BB1" s="211" t="inlineStr">
+        <is>
+          <t>GELBATTERY</t>
+        </is>
+      </c>
+      <c r="BC1" s="211" t="inlineStr">
+        <is>
+          <t>FORTIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Mine.io</t>
         </is>
       </c>
-      <c r="B2" s="137" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>FBI</t>
         </is>
       </c>
-      <c r="C2" s="137" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>liguh</t>
         </is>
       </c>
-      <c r="D2" s="138" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>2024-04-12</t>
         </is>
       </c>
-      <c r="E2" s="138" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>2024-06-15</t>
         </is>
       </c>
-      <c r="F2" s="139" t="n">
+      <c r="F2" t="n">
         <v>480</v>
       </c>
-      <c r="G2" s="137" t="n">
+      <c r="G2" t="n">
         <v>480</v>
       </c>
-      <c r="H2" s="137" t="n"/>
-      <c r="I2" s="137" t="n">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
         <v>2</v>
       </c>
-      <c r="J2" s="137" t="n">
+      <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="137" t="n"/>
-      <c r="L2" s="137" t="n"/>
-      <c r="M2" s="137" t="n"/>
-      <c r="N2" s="137" t="n"/>
-      <c r="O2" s="137" t="n"/>
-      <c r="P2" s="137" t="n"/>
-      <c r="Q2" s="137" t="n"/>
-      <c r="R2" s="137" t="n"/>
-      <c r="S2" s="137" t="n"/>
-      <c r="T2" s="137" t="n"/>
-      <c r="U2" s="137" t="n"/>
-      <c r="V2" s="137" t="n"/>
-      <c r="W2" s="137" t="n"/>
-      <c r="X2" s="137" t="n">
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="n">
         <v>3</v>
       </c>
-      <c r="Y2" s="137" t="n">
+      <c r="Y2" t="n">
         <v>3</v>
       </c>
-      <c r="Z2" s="137" t="n">
+      <c r="Z2" t="n">
         <v>3</v>
       </c>
-      <c r="AA2" s="137" t="n">
+      <c r="AA2" t="n">
         <v>3</v>
       </c>
-      <c r="AB2" s="137" t="n"/>
-      <c r="AC2" s="137" t="n">
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="n">
         <v>3</v>
       </c>
-      <c r="AD2" s="137" t="n"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" s="106">
-      <c r="A3" s="137" t="inlineStr">
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Rapakivi2</t>
         </is>
       </c>
-      <c r="B3" s="137" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>NASA</t>
         </is>
       </c>
-      <c r="C3" s="137" t="n"/>
-      <c r="D3" s="138" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ببب</t>
+        </is>
+      </c>
+      <c r="D3" s="212" t="n">
         <v>44242</v>
       </c>
-      <c r="E3" s="138" t="n">
+      <c r="E3" s="212" t="n">
         <v>45458</v>
       </c>
-      <c r="F3" s="139" t="n">
+      <c r="F3" t="n">
         <v>50</v>
       </c>
-      <c r="G3" s="137" t="n">
+      <c r="G3" t="n">
         <v>50</v>
       </c>
-      <c r="H3" s="137" t="n"/>
-      <c r="I3" s="137" t="n"/>
-      <c r="J3" s="137" t="n"/>
-      <c r="K3" s="137" t="n">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
         <v>20</v>
       </c>
-      <c r="L3" s="137" t="n"/>
-      <c r="M3" s="137" t="n"/>
-      <c r="N3" s="137" t="n"/>
-      <c r="O3" s="137" t="n"/>
-      <c r="P3" s="137" t="n"/>
-      <c r="Q3" s="137" t="n"/>
-      <c r="R3" s="137" t="n"/>
-      <c r="S3" s="137" t="n"/>
-      <c r="T3" s="137" t="n"/>
-      <c r="U3" s="137" t="n"/>
-      <c r="V3" s="137" t="n"/>
-      <c r="W3" s="137" t="n"/>
-      <c r="X3" s="137" t="n">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="n">
         <v>4</v>
       </c>
-      <c r="Y3" s="137" t="n"/>
-      <c r="Z3" s="137" t="n">
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="n">
         <v>4</v>
       </c>
-      <c r="AA3" s="137" t="n">
+      <c r="AA3" t="n">
         <v>4</v>
       </c>
-      <c r="AB3" s="137" t="n">
+      <c r="AB3" t="n">
         <v>4</v>
       </c>
-      <c r="AC3" s="137" t="n">
+      <c r="AC3" t="n">
         <v>4</v>
       </c>
-      <c r="AD3" s="137" t="n">
+      <c r="AD3" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" s="106">
-      <c r="A4" s="137" t="inlineStr">
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>REASSESS</t>
         </is>
       </c>
-      <c r="B4" s="137" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Russia</t>
         </is>
       </c>
-      <c r="C4" s="137" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>IGE (FR)</t>
         </is>
       </c>
-      <c r="D4" s="138" t="n">
+      <c r="D4" s="212" t="n">
         <v>45397</v>
       </c>
-      <c r="E4" s="138" t="n">
+      <c r="E4" s="212" t="n">
         <v>45961</v>
       </c>
-      <c r="F4" s="137" t="n">
+      <c r="F4" t="n">
         <v>120</v>
       </c>
-      <c r="G4" s="137" t="n">
+      <c r="G4" t="n">
         <v>120</v>
       </c>
-      <c r="H4" s="137" t="n"/>
-      <c r="I4" s="137" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="137" t="n"/>
-      <c r="K4" s="137" t="n">
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
         <v>15</v>
       </c>
-      <c r="L4" s="137" t="n"/>
-      <c r="M4" s="137" t="n">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="137" t="n"/>
-      <c r="O4" s="137" t="n"/>
-      <c r="P4" s="137" t="n"/>
-      <c r="Q4" s="137" t="n"/>
-      <c r="R4" s="137" t="n"/>
-      <c r="S4" s="137" t="n"/>
-      <c r="T4" s="137" t="n"/>
-      <c r="U4" s="137" t="n"/>
-      <c r="V4" s="137" t="n"/>
-      <c r="W4" s="137" t="n"/>
-      <c r="X4" s="137" t="n"/>
-      <c r="Y4" s="137" t="n"/>
-      <c r="Z4" s="137" t="n"/>
-      <c r="AA4" s="137" t="n"/>
-      <c r="AB4" s="137" t="n"/>
-      <c r="AC4" s="137" t="n"/>
-      <c r="AD4" s="137" t="n"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="106">
-      <c r="A5" s="137" t="inlineStr">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>GRANDE</t>
         </is>
       </c>
-      <c r="B5" s="137" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Grand Canyon</t>
         </is>
       </c>
-      <c r="C5" s="137" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>INGV; U Padova</t>
         </is>
       </c>
-      <c r="D5" s="138" t="n">
+      <c r="D5" s="212" t="n">
         <v>45407</v>
       </c>
-      <c r="E5" s="138" t="n">
+      <c r="E5" s="212" t="n">
         <v>45493</v>
       </c>
-      <c r="F5" s="137" t="n">
+      <c r="F5" t="n">
         <v>170</v>
       </c>
-      <c r="G5" s="137" t="n">
+      <c r="G5" t="n">
         <v>170</v>
       </c>
-      <c r="H5" s="137" t="n"/>
-      <c r="I5" s="137" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="137" t="n"/>
-      <c r="K5" s="137" t="n"/>
-      <c r="L5" s="137" t="n"/>
-      <c r="M5" s="137" t="n"/>
-      <c r="N5" s="137" t="n"/>
-      <c r="O5" s="137" t="n"/>
-      <c r="P5" s="137" t="n"/>
-      <c r="Q5" s="137" t="n"/>
-      <c r="R5" s="137" t="n"/>
-      <c r="S5" s="137" t="n"/>
-      <c r="T5" s="137" t="n"/>
-      <c r="U5" s="137" t="n"/>
-      <c r="V5" s="137" t="n"/>
-      <c r="W5" s="137" t="n"/>
-      <c r="X5" s="137" t="n"/>
-      <c r="Y5" s="137" t="n"/>
-      <c r="Z5" s="137" t="n"/>
-      <c r="AA5" s="137" t="n"/>
-      <c r="AB5" s="137" t="n"/>
-      <c r="AC5" s="137" t="n"/>
-      <c r="AD5" s="137" t="n"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" s="106">
-      <c r="A6" s="137" t="inlineStr">
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>ThermEcoWat</t>
         </is>
       </c>
-      <c r="B6" s="137" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>NBA</t>
         </is>
       </c>
-      <c r="C6" s="137" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Roma</t>
         </is>
       </c>
-      <c r="D6" s="138" t="n"/>
-      <c r="E6" s="138" t="n"/>
-      <c r="F6" s="137" t="n"/>
-      <c r="G6" s="137" t="n"/>
-      <c r="H6" s="137" t="n"/>
-      <c r="I6" s="137" t="n"/>
-      <c r="J6" s="137" t="n"/>
-      <c r="K6" s="137" t="n"/>
-      <c r="L6" s="137" t="n"/>
-      <c r="M6" s="137" t="n"/>
-      <c r="N6" s="137" t="n"/>
-      <c r="O6" s="137" t="n"/>
-      <c r="P6" s="137" t="n"/>
-      <c r="Q6" s="137" t="n"/>
-      <c r="R6" s="137" t="n"/>
-      <c r="S6" s="137" t="n"/>
-      <c r="T6" s="137" t="n"/>
-      <c r="U6" s="137" t="n"/>
-      <c r="V6" s="137" t="n"/>
-      <c r="W6" s="137" t="n"/>
-      <c r="X6" s="137" t="n"/>
-      <c r="Y6" s="137" t="n"/>
-      <c r="Z6" s="137" t="n"/>
-      <c r="AA6" s="137" t="n"/>
-      <c r="AB6" s="137" t="n"/>
-      <c r="AC6" s="137" t="n"/>
-      <c r="AD6" s="137" t="n"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" s="106">
-      <c r="A7" s="137" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Geoenergialoikka</t>
         </is>
       </c>
-      <c r="B7" s="137" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="C7" s="137" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Ohaio</t>
         </is>
       </c>
-      <c r="D7" s="138" t="n">
+      <c r="D7" s="212" t="n">
         <v>45558</v>
       </c>
-      <c r="E7" s="138" t="n">
+      <c r="E7" s="212" t="n">
         <v>45618</v>
       </c>
-      <c r="F7" s="137" t="n">
+      <c r="F7" t="n">
         <v>900</v>
       </c>
-      <c r="G7" s="137" t="n">
+      <c r="G7" t="n">
         <v>900</v>
       </c>
-      <c r="H7" s="137" t="n"/>
-      <c r="I7" s="137" t="n"/>
-      <c r="J7" s="137" t="n">
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="137" t="n"/>
-      <c r="L7" s="137" t="n"/>
-      <c r="M7" s="137" t="n"/>
-      <c r="N7" s="137" t="n"/>
-      <c r="O7" s="137" t="n"/>
-      <c r="P7" s="137" t="n"/>
-      <c r="Q7" s="137" t="n"/>
-      <c r="R7" s="137" t="n"/>
-      <c r="S7" s="137" t="n"/>
-      <c r="T7" s="137" t="n"/>
-      <c r="U7" s="137" t="n"/>
-      <c r="V7" s="137" t="n"/>
-      <c r="W7" s="137" t="n"/>
-      <c r="X7" s="137" t="n"/>
-      <c r="Y7" s="137" t="n"/>
-      <c r="Z7" s="137" t="n"/>
-      <c r="AA7" s="137" t="n"/>
-      <c r="AB7" s="137" t="n"/>
-      <c r="AC7" s="137" t="n"/>
-      <c r="AD7" s="137" t="n"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" s="106">
-      <c r="A8" s="137" t="inlineStr">
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="inlineStr"/>
+      <c r="AW7" t="inlineStr"/>
+      <c r="AX7" t="inlineStr"/>
+      <c r="AY7" t="inlineStr"/>
+      <c r="AZ7" t="inlineStr"/>
+      <c r="BA7" t="inlineStr"/>
+      <c r="BB7" t="inlineStr"/>
+      <c r="BC7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>LINK-FEUT2</t>
         </is>
       </c>
-      <c r="B8" s="137" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C8" s="137" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>morroco</t>
         </is>
       </c>
-      <c r="D8" s="138" t="n">
+      <c r="D8" s="212" t="n">
         <v>45536</v>
       </c>
-      <c r="E8" s="138" t="n">
+      <c r="E8" s="212" t="n">
         <v>45564</v>
       </c>
-      <c r="F8" s="137" t="n">
+      <c r="F8" t="n">
         <v>80</v>
       </c>
-      <c r="G8" s="137" t="n">
+      <c r="G8" t="n">
         <v>80</v>
       </c>
-      <c r="H8" s="137" t="n"/>
-      <c r="I8" s="137" t="n">
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="137" t="n"/>
-      <c r="K8" s="137" t="n"/>
-      <c r="L8" s="137" t="n"/>
-      <c r="M8" s="137" t="n"/>
-      <c r="N8" s="137" t="n"/>
-      <c r="O8" s="137" t="n"/>
-      <c r="P8" s="137" t="n"/>
-      <c r="Q8" s="137" t="n"/>
-      <c r="R8" s="137" t="n"/>
-      <c r="S8" s="137" t="n"/>
-      <c r="T8" s="137" t="n"/>
-      <c r="U8" s="137" t="n"/>
-      <c r="V8" s="137" t="n"/>
-      <c r="W8" s="137" t="n"/>
-      <c r="X8" s="137" t="n"/>
-      <c r="Y8" s="137" t="n"/>
-      <c r="Z8" s="137" t="n"/>
-      <c r="AA8" s="137" t="n"/>
-      <c r="AB8" s="137" t="n"/>
-      <c r="AC8" s="137" t="n"/>
-      <c r="AD8" s="137" t="n"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1" s="106">
-      <c r="A9" s="137" t="inlineStr">
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>AdriaArray</t>
         </is>
       </c>
-      <c r="B9" s="137" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C9" s="137" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>France</t>
         </is>
       </c>
-      <c r="D9" s="138" t="n">
+      <c r="D9" s="212" t="n">
         <v>44713</v>
       </c>
-      <c r="E9" s="138" t="n">
+      <c r="E9" s="212" t="n">
         <v>45534</v>
       </c>
-      <c r="F9" s="137" t="n"/>
-      <c r="G9" s="137" t="n"/>
-      <c r="H9" s="137" t="n"/>
-      <c r="I9" s="137" t="n"/>
-      <c r="J9" s="137" t="n"/>
-      <c r="K9" s="137" t="n"/>
-      <c r="L9" s="137" t="n"/>
-      <c r="M9" s="137" t="n"/>
-      <c r="N9" s="137" t="n"/>
-      <c r="O9" s="137" t="n"/>
-      <c r="P9" s="137" t="n"/>
-      <c r="Q9" s="137" t="n"/>
-      <c r="R9" s="137" t="n"/>
-      <c r="S9" s="137" t="n"/>
-      <c r="T9" s="137" t="n"/>
-      <c r="U9" s="137" t="n"/>
-      <c r="V9" s="137" t="n"/>
-      <c r="W9" s="137" t="n"/>
-      <c r="X9" s="137" t="n">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="n">
         <v>20</v>
       </c>
-      <c r="Y9" s="137" t="n">
+      <c r="Y9" t="n">
         <v>20</v>
       </c>
-      <c r="Z9" s="137" t="n">
+      <c r="Z9" t="n">
         <v>20</v>
       </c>
-      <c r="AA9" s="137" t="n">
+      <c r="AA9" t="n">
         <v>20</v>
       </c>
-      <c r="AB9" s="137" t="n">
+      <c r="AB9" t="n">
         <v>20</v>
       </c>
-      <c r="AC9" s="137" t="n">
+      <c r="AC9" t="n">
         <v>20</v>
       </c>
-      <c r="AD9" s="137" t="n"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="106">
-      <c r="A10" s="137" t="inlineStr">
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>AdriaArray2</t>
         </is>
       </c>
-      <c r="B10" s="137" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C10" s="137" t="n"/>
-      <c r="D10" s="138" t="n">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" s="212" t="n">
         <v>45536</v>
       </c>
-      <c r="E10" s="138" t="n">
+      <c r="E10" s="212" t="n">
         <v>45930</v>
       </c>
-      <c r="F10" s="137" t="n"/>
-      <c r="G10" s="137" t="n"/>
-      <c r="H10" s="137" t="n"/>
-      <c r="I10" s="137" t="n"/>
-      <c r="J10" s="137" t="n"/>
-      <c r="K10" s="137" t="n"/>
-      <c r="L10" s="137" t="n"/>
-      <c r="M10" s="137" t="n"/>
-      <c r="N10" s="137" t="n"/>
-      <c r="O10" s="137" t="n"/>
-      <c r="P10" s="137" t="n"/>
-      <c r="Q10" s="137" t="n"/>
-      <c r="R10" s="137" t="n"/>
-      <c r="S10" s="137" t="n"/>
-      <c r="T10" s="137" t="n"/>
-      <c r="U10" s="137" t="n"/>
-      <c r="V10" s="137" t="n"/>
-      <c r="W10" s="137" t="n"/>
-      <c r="X10" s="137" t="n">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="n">
         <v>20</v>
       </c>
-      <c r="Y10" s="137" t="n">
+      <c r="Y10" t="n">
         <v>20</v>
       </c>
-      <c r="Z10" s="137" t="n">
+      <c r="Z10" t="n">
         <v>20</v>
       </c>
-      <c r="AA10" s="137" t="n">
+      <c r="AA10" t="n">
         <v>20</v>
       </c>
-      <c r="AB10" s="137" t="n">
+      <c r="AB10" t="n">
         <v>20</v>
       </c>
-      <c r="AC10" s="137" t="n">
+      <c r="AC10" t="n">
         <v>20</v>
       </c>
-      <c r="AD10" s="137" t="n"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1" s="106">
-      <c r="A11" s="137" t="inlineStr">
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="inlineStr"/>
+      <c r="BA10" t="inlineStr"/>
+      <c r="BB10" t="inlineStr"/>
+      <c r="BC10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>SCARCE</t>
         </is>
       </c>
-      <c r="B11" s="137" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C11" s="137" t="n"/>
-      <c r="D11" s="138" t="n">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" s="212" t="n">
         <v>44819</v>
       </c>
-      <c r="E11" s="138" t="n">
+      <c r="E11" s="212" t="n">
         <v>45550</v>
       </c>
-      <c r="F11" s="137" t="n"/>
-      <c r="G11" s="137" t="n"/>
-      <c r="H11" s="137" t="n"/>
-      <c r="I11" s="137" t="n"/>
-      <c r="J11" s="137" t="n"/>
-      <c r="K11" s="137" t="n"/>
-      <c r="L11" s="137" t="n"/>
-      <c r="M11" s="137" t="n"/>
-      <c r="N11" s="137" t="n"/>
-      <c r="O11" s="137" t="n"/>
-      <c r="P11" s="137" t="n"/>
-      <c r="Q11" s="137" t="n"/>
-      <c r="R11" s="137" t="n"/>
-      <c r="S11" s="137" t="n"/>
-      <c r="T11" s="137" t="n"/>
-      <c r="U11" s="137" t="n"/>
-      <c r="V11" s="137" t="n"/>
-      <c r="W11" s="137" t="n"/>
-      <c r="X11" s="137" t="n">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="n">
         <v>10</v>
       </c>
-      <c r="Y11" s="137" t="n">
+      <c r="Y11" t="n">
         <v>10</v>
       </c>
-      <c r="Z11" s="137" t="n">
+      <c r="Z11" t="n">
         <v>10</v>
       </c>
-      <c r="AA11" s="137" t="n">
+      <c r="AA11" t="n">
         <v>10</v>
       </c>
-      <c r="AB11" s="137" t="n">
+      <c r="AB11" t="n">
         <v>10</v>
       </c>
-      <c r="AC11" s="137" t="n">
+      <c r="AC11" t="n">
         <v>10</v>
       </c>
-      <c r="AD11" s="137" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" s="106">
-      <c r="A12" s="137" t="inlineStr">
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr"/>
+      <c r="AW11" t="inlineStr"/>
+      <c r="AX11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr"/>
+      <c r="AZ11" t="inlineStr"/>
+      <c r="BA11" t="inlineStr"/>
+      <c r="BB11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Oulu equipment testssssss</t>
         </is>
       </c>
-      <c r="B12" s="137" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>UOULU</t>
         </is>
       </c>
-      <c r="C12" s="137" t="n"/>
-      <c r="D12" s="138" t="n">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" s="212" t="n">
         <v>45323</v>
       </c>
-      <c r="E12" s="138" t="n">
+      <c r="E12" s="212" t="n">
         <v>45657</v>
       </c>
-      <c r="F12" s="137" t="n"/>
-      <c r="G12" s="137" t="n">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
         <v>50</v>
       </c>
-      <c r="H12" s="137" t="n">
+      <c r="H12" t="n">
         <v>50</v>
       </c>
-      <c r="I12" s="137" t="n">
+      <c r="I12" t="n">
         <v>2</v>
       </c>
-      <c r="J12" s="137" t="n"/>
-      <c r="K12" s="137" t="n"/>
-      <c r="L12" s="137" t="n">
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
         <v>50</v>
       </c>
-      <c r="M12" s="137" t="n"/>
-      <c r="N12" s="137" t="n">
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="n">
         <v>1</v>
       </c>
-      <c r="O12" s="137" t="n"/>
-      <c r="P12" s="137" t="n">
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
         <v>2</v>
       </c>
-      <c r="Q12" s="137" t="n">
+      <c r="Q12" t="n">
         <v>1</v>
       </c>
-      <c r="R12" s="137" t="n">
+      <c r="R12" t="n">
         <v>1</v>
       </c>
-      <c r="S12" s="137" t="n"/>
-      <c r="T12" s="137" t="n"/>
-      <c r="U12" s="137" t="n"/>
-      <c r="V12" s="137" t="n"/>
-      <c r="W12" s="137" t="n"/>
-      <c r="X12" s="137" t="n"/>
-      <c r="Y12" s="137" t="n"/>
-      <c r="Z12" s="137" t="n"/>
-      <c r="AA12" s="137" t="n"/>
-      <c r="AB12" s="137" t="n"/>
-      <c r="AC12" s="137" t="n"/>
-      <c r="AD12" s="137" t="n"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" s="106">
-      <c r="A13" s="137" t="inlineStr">
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
+      <c r="AT12" t="inlineStr"/>
+      <c r="AU12" t="inlineStr"/>
+      <c r="AV12" t="inlineStr"/>
+      <c r="AW12" t="inlineStr"/>
+      <c r="AX12" t="inlineStr"/>
+      <c r="AY12" t="inlineStr"/>
+      <c r="AZ12" t="inlineStr"/>
+      <c r="BA12" t="inlineStr"/>
+      <c r="BB12" t="inlineStr"/>
+      <c r="BC12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>kir</t>
         </is>
       </c>
-      <c r="B13" s="137" t="n"/>
-      <c r="C13" s="137" t="n"/>
-      <c r="D13" s="138" t="n"/>
-      <c r="E13" s="138" t="n"/>
-      <c r="F13" s="137" t="n"/>
-      <c r="G13" s="137" t="n"/>
-      <c r="H13" s="137" t="n"/>
-      <c r="I13" s="137" t="n"/>
-      <c r="J13" s="137" t="n"/>
-      <c r="K13" s="137" t="n"/>
-      <c r="L13" s="137" t="n"/>
-      <c r="M13" s="137" t="n"/>
-      <c r="N13" s="137" t="n"/>
-      <c r="O13" s="137" t="n"/>
-      <c r="P13" s="137" t="n"/>
-      <c r="Q13" s="137" t="n"/>
-      <c r="R13" s="137" t="n"/>
-      <c r="S13" s="137" t="n"/>
-      <c r="T13" s="137" t="n"/>
-      <c r="U13" s="137" t="n"/>
-      <c r="V13" s="137" t="n"/>
-      <c r="W13" s="137" t="n"/>
-      <c r="X13" s="137" t="n"/>
-      <c r="Y13" s="137" t="n"/>
-      <c r="Z13" s="137" t="n"/>
-      <c r="AA13" s="137" t="n"/>
-      <c r="AB13" s="137" t="n"/>
-      <c r="AC13" s="137" t="n"/>
-      <c r="AD13" s="137" t="n"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="106">
-      <c r="A14" s="137" t="inlineStr">
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr"/>
+      <c r="AV13" t="inlineStr"/>
+      <c r="AW13" t="inlineStr"/>
+      <c r="AX13" t="inlineStr"/>
+      <c r="AY13" t="inlineStr"/>
+      <c r="AZ13" t="inlineStr"/>
+      <c r="BA13" t="inlineStr"/>
+      <c r="BB13" t="inlineStr"/>
+      <c r="BC13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>DYNALake</t>
         </is>
       </c>
-      <c r="B14" s="137" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C14" s="137" t="n"/>
-      <c r="D14" s="138" t="n">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" s="212" t="n">
         <v>45586</v>
       </c>
-      <c r="E14" s="138" t="n">
+      <c r="E14" s="212" t="n">
         <v>45808</v>
       </c>
-      <c r="F14" s="137" t="n">
+      <c r="F14" t="n">
         <v>40</v>
       </c>
-      <c r="G14" s="137" t="n">
+      <c r="G14" t="n">
         <v>40</v>
       </c>
-      <c r="H14" s="137" t="n"/>
-      <c r="I14" s="137" t="n">
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
         <v>3</v>
       </c>
-      <c r="J14" s="137" t="n"/>
-      <c r="K14" s="137" t="n"/>
-      <c r="L14" s="137" t="n">
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="n">
         <v>40</v>
       </c>
-      <c r="M14" s="137" t="n"/>
-      <c r="N14" s="137" t="n"/>
-      <c r="O14" s="137" t="n"/>
-      <c r="P14" s="137" t="n"/>
-      <c r="Q14" s="137" t="n"/>
-      <c r="R14" s="137" t="n"/>
-      <c r="S14" s="137" t="n"/>
-      <c r="T14" s="137" t="n"/>
-      <c r="U14" s="137" t="n"/>
-      <c r="V14" s="137" t="n"/>
-      <c r="W14" s="137" t="n"/>
-      <c r="X14" s="137" t="n"/>
-      <c r="Y14" s="137" t="n"/>
-      <c r="Z14" s="137" t="n"/>
-      <c r="AA14" s="137" t="n"/>
-      <c r="AB14" s="137" t="n"/>
-      <c r="AC14" s="137" t="n"/>
-      <c r="AD14" s="137" t="n"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" s="106">
-      <c r="A15" s="137" t="inlineStr">
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr"/>
+      <c r="AV14" t="inlineStr"/>
+      <c r="AW14" t="inlineStr"/>
+      <c r="AX14" t="inlineStr"/>
+      <c r="AY14" t="inlineStr"/>
+      <c r="AZ14" t="inlineStr"/>
+      <c r="BA14" t="inlineStr"/>
+      <c r="BB14" t="inlineStr"/>
+      <c r="BC14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>DYNALake</t>
         </is>
       </c>
-      <c r="B15" s="137" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C15" s="137" t="n"/>
-      <c r="D15" s="138" t="inlineStr">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
         <is>
           <t>2025-01-15</t>
         </is>
       </c>
-      <c r="E15" s="138" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>2025-04-03</t>
         </is>
       </c>
-      <c r="F15" s="137" t="n">
+      <c r="F15" t="n">
         <v>356</v>
       </c>
-      <c r="G15" s="137" t="n">
+      <c r="G15" t="n">
         <v>350</v>
       </c>
-      <c r="H15" s="137" t="n"/>
-      <c r="I15" s="137" t="n"/>
-      <c r="J15" s="137" t="n">
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
         <v>1</v>
       </c>
-      <c r="K15" s="137" t="n"/>
-      <c r="L15" s="137" t="n"/>
-      <c r="M15" s="137" t="n"/>
-      <c r="N15" s="137" t="n"/>
-      <c r="O15" s="137" t="n"/>
-      <c r="P15" s="137" t="n"/>
-      <c r="Q15" s="137" t="n"/>
-      <c r="R15" s="137" t="n"/>
-      <c r="S15" s="137" t="n"/>
-      <c r="T15" s="137" t="n"/>
-      <c r="U15" s="137" t="n"/>
-      <c r="V15" s="137" t="n"/>
-      <c r="W15" s="137" t="n">
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="n">
         <v>1</v>
       </c>
-      <c r="X15" s="137" t="n"/>
-      <c r="Y15" s="137" t="n"/>
-      <c r="Z15" s="137" t="n"/>
-      <c r="AA15" s="137" t="n"/>
-      <c r="AB15" s="137" t="n"/>
-      <c r="AC15" s="137" t="n"/>
-      <c r="AD15" s="137" t="n"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1" s="106">
-      <c r="A16" s="137" t="inlineStr">
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="inlineStr"/>
+      <c r="AV15" t="inlineStr"/>
+      <c r="AW15" t="inlineStr"/>
+      <c r="AX15" t="inlineStr"/>
+      <c r="AY15" t="inlineStr"/>
+      <c r="AZ15" t="inlineStr"/>
+      <c r="BA15" t="inlineStr"/>
+      <c r="BB15" t="inlineStr"/>
+      <c r="BC15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Semacret3</t>
         </is>
       </c>
-      <c r="B16" s="137" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>UOULU</t>
         </is>
       </c>
-      <c r="C16" s="137" t="n"/>
-      <c r="D16" s="138" t="n">
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" s="212" t="n">
         <v>45526</v>
       </c>
-      <c r="E16" s="138" t="n">
+      <c r="E16" s="212" t="n">
         <v>45581</v>
       </c>
-      <c r="F16" s="137" t="n">
+      <c r="F16" t="n">
         <v>40</v>
       </c>
-      <c r="G16" s="137" t="n">
+      <c r="G16" t="n">
         <v>40</v>
       </c>
-      <c r="H16" s="137" t="n"/>
-      <c r="I16" s="137" t="n"/>
-      <c r="J16" s="137" t="n"/>
-      <c r="K16" s="137" t="n"/>
-      <c r="L16" s="137" t="n"/>
-      <c r="M16" s="137" t="n"/>
-      <c r="N16" s="137" t="n"/>
-      <c r="O16" s="137" t="n"/>
-      <c r="P16" s="137" t="n"/>
-      <c r="Q16" s="137" t="n"/>
-      <c r="R16" s="137" t="n"/>
-      <c r="S16" s="137" t="n">
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="n">
         <v>70</v>
       </c>
-      <c r="T16" s="137" t="n"/>
-      <c r="U16" s="137" t="n">
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="n">
         <v>2</v>
       </c>
-      <c r="V16" s="137" t="n">
+      <c r="V16" t="n">
         <v>2</v>
       </c>
-      <c r="W16" s="137" t="n"/>
-      <c r="X16" s="137" t="n">
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="n">
         <v>3</v>
       </c>
-      <c r="Y16" s="137" t="n">
+      <c r="Y16" t="n">
         <v>3</v>
       </c>
-      <c r="Z16" s="137" t="n">
+      <c r="Z16" t="n">
         <v>3</v>
       </c>
-      <c r="AA16" s="137" t="n">
+      <c r="AA16" t="n">
         <v>3</v>
       </c>
-      <c r="AB16" s="137" t="n"/>
-      <c r="AC16" s="137" t="n"/>
-      <c r="AD16" s="137" t="n"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1" s="106">
-      <c r="A17" s="137" t="inlineStr">
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
+      <c r="AV16" t="inlineStr"/>
+      <c r="AW16" t="inlineStr"/>
+      <c r="AX16" t="inlineStr"/>
+      <c r="AY16" t="inlineStr"/>
+      <c r="AZ16" t="inlineStr"/>
+      <c r="BA16" t="inlineStr"/>
+      <c r="BB16" t="inlineStr"/>
+      <c r="BC16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>LINK-FINUNI</t>
         </is>
       </c>
-      <c r="B17" s="137" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="C17" s="137" t="n"/>
-      <c r="D17" s="138" t="n">
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" s="212" t="n">
         <v>45901</v>
       </c>
-      <c r="E17" s="138" t="n">
+      <c r="E17" s="212" t="n">
         <v>45919</v>
       </c>
-      <c r="F17" s="137" t="n">
+      <c r="F17" t="n">
         <v>80</v>
       </c>
-      <c r="G17" s="137" t="n">
+      <c r="G17" t="n">
         <v>80</v>
       </c>
-      <c r="H17" s="137" t="n"/>
-      <c r="I17" s="137" t="n">
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
         <v>1</v>
       </c>
-      <c r="J17" s="137" t="n">
+      <c r="J17" t="n">
         <v>1</v>
       </c>
-      <c r="K17" s="137" t="n"/>
-      <c r="L17" s="137" t="n"/>
-      <c r="M17" s="137" t="n"/>
-      <c r="N17" s="137" t="n"/>
-      <c r="O17" s="137" t="n"/>
-      <c r="P17" s="137" t="n"/>
-      <c r="Q17" s="137" t="n"/>
-      <c r="R17" s="137" t="n"/>
-      <c r="S17" s="137" t="n"/>
-      <c r="T17" s="137" t="n"/>
-      <c r="U17" s="137" t="n"/>
-      <c r="V17" s="137" t="n"/>
-      <c r="W17" s="137" t="n"/>
-      <c r="X17" s="137" t="n"/>
-      <c r="Y17" s="137" t="n"/>
-      <c r="Z17" s="137" t="n"/>
-      <c r="AA17" s="137" t="n"/>
-      <c r="AB17" s="137" t="n"/>
-      <c r="AC17" s="137" t="n"/>
-      <c r="AD17" s="137" t="n"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1" s="106">
-      <c r="A18" s="137" t="inlineStr">
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
+      <c r="AS17" t="inlineStr"/>
+      <c r="AT17" t="inlineStr"/>
+      <c r="AU17" t="inlineStr"/>
+      <c r="AV17" t="inlineStr"/>
+      <c r="AW17" t="inlineStr"/>
+      <c r="AX17" t="inlineStr"/>
+      <c r="AY17" t="inlineStr"/>
+      <c r="AZ17" t="inlineStr"/>
+      <c r="BA17" t="inlineStr"/>
+      <c r="BB17" t="inlineStr"/>
+      <c r="BC17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Mine.io2</t>
         </is>
       </c>
-      <c r="B18" s="137" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>UOULU</t>
         </is>
       </c>
-      <c r="C18" s="137" t="n"/>
-      <c r="D18" s="138" t="n">
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" s="212" t="n">
         <v>45578</v>
       </c>
-      <c r="E18" s="138" t="n">
+      <c r="E18" s="212" t="n">
         <v>45777</v>
       </c>
-      <c r="F18" s="137" t="n">
+      <c r="F18" t="n">
         <v>80</v>
       </c>
-      <c r="G18" s="137" t="n">
+      <c r="G18" t="n">
         <v>80</v>
       </c>
-      <c r="H18" s="137" t="n"/>
-      <c r="I18" s="137" t="n">
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
         <v>1</v>
       </c>
-      <c r="J18" s="137" t="n"/>
-      <c r="K18" s="137" t="n"/>
-      <c r="L18" s="137" t="n"/>
-      <c r="M18" s="137" t="n"/>
-      <c r="N18" s="137" t="n"/>
-      <c r="O18" s="137" t="n"/>
-      <c r="P18" s="137" t="n"/>
-      <c r="Q18" s="137" t="n"/>
-      <c r="R18" s="137" t="n"/>
-      <c r="S18" s="137" t="n"/>
-      <c r="T18" s="137" t="n"/>
-      <c r="U18" s="137" t="n"/>
-      <c r="V18" s="137" t="n"/>
-      <c r="W18" s="137" t="n"/>
-      <c r="X18" s="137" t="n">
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="n">
         <v>3</v>
       </c>
-      <c r="Y18" s="137" t="n">
+      <c r="Y18" t="n">
         <v>3</v>
       </c>
-      <c r="Z18" s="137" t="n">
+      <c r="Z18" t="n">
         <v>3</v>
       </c>
-      <c r="AA18" s="137" t="n">
+      <c r="AA18" t="n">
         <v>3</v>
       </c>
-      <c r="AB18" s="137" t="n">
+      <c r="AB18" t="n">
         <v>3</v>
       </c>
-      <c r="AC18" s="137" t="n">
+      <c r="AC18" t="n">
         <v>3</v>
       </c>
-      <c r="AD18" s="137" t="n"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1" s="106">
-      <c r="A19" s="137" t="inlineStr">
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr"/>
+      <c r="AS18" t="inlineStr"/>
+      <c r="AT18" t="inlineStr"/>
+      <c r="AU18" t="inlineStr"/>
+      <c r="AV18" t="inlineStr"/>
+      <c r="AW18" t="inlineStr"/>
+      <c r="AX18" t="inlineStr"/>
+      <c r="AY18" t="inlineStr"/>
+      <c r="AZ18" t="inlineStr"/>
+      <c r="BA18" t="inlineStr"/>
+      <c r="BB18" t="inlineStr"/>
+      <c r="BC18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>UNDERCOVER</t>
         </is>
       </c>
-      <c r="B19" s="137" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="C19" s="137" t="n"/>
-      <c r="D19" s="138" t="n">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" s="212" t="n">
         <v>45809</v>
       </c>
-      <c r="E19" s="138" t="n">
+      <c r="E19" s="212" t="n">
         <v>45879</v>
       </c>
-      <c r="F19" s="137" t="n">
+      <c r="F19" t="n">
         <v>1000</v>
       </c>
-      <c r="G19" s="137" t="n">
+      <c r="G19" t="n">
         <v>500</v>
       </c>
-      <c r="H19" s="137" t="n"/>
-      <c r="I19" s="137" t="n">
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
         <v>4</v>
       </c>
-      <c r="J19" s="137" t="n">
+      <c r="J19" t="n">
         <v>1</v>
       </c>
-      <c r="K19" s="137" t="n"/>
-      <c r="L19" s="137" t="n"/>
-      <c r="M19" s="137" t="n"/>
-      <c r="N19" s="137" t="n"/>
-      <c r="O19" s="137" t="n"/>
-      <c r="P19" s="137" t="n"/>
-      <c r="Q19" s="137" t="n"/>
-      <c r="R19" s="137" t="n"/>
-      <c r="S19" s="137" t="n"/>
-      <c r="T19" s="137" t="n"/>
-      <c r="U19" s="137" t="n"/>
-      <c r="V19" s="137" t="n"/>
-      <c r="W19" s="137" t="n"/>
-      <c r="X19" s="137" t="n"/>
-      <c r="Y19" s="137" t="n"/>
-      <c r="Z19" s="137" t="n"/>
-      <c r="AA19" s="137" t="n"/>
-      <c r="AB19" s="137" t="n"/>
-      <c r="AC19" s="137" t="n"/>
-      <c r="AD19" s="137" t="n"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
+      <c r="AS19" t="inlineStr"/>
+      <c r="AT19" t="inlineStr"/>
+      <c r="AU19" t="inlineStr"/>
+      <c r="AV19" t="inlineStr"/>
+      <c r="AW19" t="inlineStr"/>
+      <c r="AX19" t="inlineStr"/>
+      <c r="AY19" t="inlineStr"/>
+      <c r="AZ19" t="inlineStr"/>
+      <c r="BA19" t="inlineStr"/>
+      <c r="BB19" t="inlineStr"/>
+      <c r="BC19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DYNALake</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" s="212" t="n">
+        <v>45561</v>
+      </c>
+      <c r="E20" s="212" t="n">
+        <v>45674</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr"/>
+      <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr"/>
+      <c r="AS20" t="inlineStr"/>
+      <c r="AT20" t="inlineStr"/>
+      <c r="AU20" t="inlineStr"/>
+      <c r="AV20" t="inlineStr"/>
+      <c r="AW20" t="inlineStr"/>
+      <c r="AX20" t="inlineStr"/>
+      <c r="AY20" t="inlineStr"/>
+      <c r="AZ20" t="inlineStr"/>
+      <c r="BA20" t="inlineStr"/>
+      <c r="BB20" t="inlineStr"/>
+      <c r="BC20" t="inlineStr"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
delete row added to tables
</commit_message>
<xml_diff>
--- a/data/pool.xlsx
+++ b/data/pool.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\inventory\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\seismo_inventory_management\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E89293F-1986-45AE-A27D-07ED93441CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A24A34-F07F-40EC-B78D-3E9D9C8EAF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -38,7 +41,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>None</author>
+    <author/>
   </authors>
   <commentList>
     <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="111">
   <si>
     <t>Projects</t>
   </si>
@@ -153,7 +156,7 @@
     <t>FORTIS</t>
   </si>
   <si>
-    <t>Mineddd.io</t>
+    <t>Mine.io</t>
   </si>
   <si>
     <t>FBI</t>
@@ -205,12 +208,6 @@
   </si>
   <si>
     <t>california</t>
-  </si>
-  <si>
-    <t>2024-09-20</t>
-  </si>
-  <si>
-    <t>2027-06-15</t>
   </si>
   <si>
     <t>LINK-FEUT2</t>
@@ -861,12 +858,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pivot Table Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Pivot Table Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Pivot Table Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Pivot Table Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Pivot Table Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Pivot Table Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Pivot Table Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Pivot Table Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Pivot Table Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Pivot Table Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Pivot Table Title" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Pivot Table Value" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -960,44 +957,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1024,14 +1021,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1058,6 +1073,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1069,166 +1102,162 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -1236,17 +1265,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="45.44140625" customWidth="1"/>
-    <col min="5" max="5" width="68.44140625" customWidth="1"/>
+    <col min="4" max="5" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="13.8" customHeight="1">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" customHeight="1">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1382,7 +1410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" customHeight="1">
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1426,7 +1454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1">
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1458,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1484,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1501,7 +1529,7 @@
         <v>45493</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1511,11 +1539,11 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
+      <c r="D7" s="3">
+        <v>45558</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45618</v>
       </c>
       <c r="F7">
         <v>900</v>
@@ -1527,15 +1555,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15" customHeight="1">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
       </c>
       <c r="D8" s="3">
         <v>45536</v>
@@ -1553,15 +1581,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15" customHeight="1">
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3">
         <v>44713</v>
@@ -1588,15 +1616,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" customHeight="1">
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3">
         <v>45536</v>
@@ -1623,12 +1651,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="15" customHeight="1">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3">
         <v>44819</v>
@@ -1655,15 +1683,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="15" customHeight="1">
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
         <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
       </c>
       <c r="D12" s="3">
         <v>45323</v>
@@ -1696,26 +1724,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="15" customHeight="1">
+    <row r="13" spans="1:30">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3">
         <v>45323</v>
       </c>
       <c r="E13" s="3">
-        <v>45657</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="15" customHeight="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3">
         <v>45586</v>
@@ -1736,21 +1764,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="15" customHeight="1">
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" s="3">
-        <v>45586</v>
+        <v>45323</v>
       </c>
       <c r="E15" s="3">
-        <v>45808</v>
+        <v>45919</v>
       </c>
       <c r="F15">
         <v>356</v>
@@ -1765,12 +1793,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="15" customHeight="1">
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="3">
         <v>45526</v>
@@ -1806,12 +1834,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="15" customHeight="1">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3">
         <v>45901</v>
@@ -1832,12 +1860,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15" customHeight="1">
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3">
         <v>45578</v>
@@ -1873,9 +1901,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15" customHeight="1">
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
@@ -1899,9 +1927,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15" customHeight="1">
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3">
         <v>45561</v>
@@ -1920,7 +1948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
@@ -1934,28 +1964,28 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>24</v>
@@ -1967,15 +1997,15 @@
         <v>46</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>15</v>
@@ -1987,15 +2017,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>15</v>
@@ -2007,15 +2037,15 @@
         <v>2</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>10</v>
@@ -2027,15 +2057,15 @@
         <v>25</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>10</v>
@@ -2047,15 +2077,15 @@
         <v>70</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>11</v>
@@ -2067,15 +2097,15 @@
         <v>50</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>26</v>
@@ -2087,15 +2117,15 @@
         <v>46</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>14</v>
@@ -2107,15 +2137,15 @@
         <v>324</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>13</v>
@@ -2127,15 +2157,15 @@
         <v>1</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>12</v>
@@ -2147,15 +2177,15 @@
         <v>2</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>12</v>
@@ -2170,12 +2200,12 @@
         <v>46</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>12</v>
@@ -2187,15 +2217,15 @@
         <v>1</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>12</v>
@@ -2207,15 +2237,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>29</v>
@@ -2227,15 +2257,15 @@
         <v>5</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>28</v>
@@ -2247,15 +2277,15 @@
         <v>20</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>25</v>
@@ -2267,15 +2297,15 @@
         <v>46</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>5</v>
@@ -2288,15 +2318,15 @@
         <v>412</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>5</v>
@@ -2311,12 +2341,12 @@
         <v>46</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>5</v>
@@ -2329,15 +2359,15 @@
         <v>185</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>5</v>
@@ -2349,15 +2379,15 @@
         <v>118</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>6</v>
@@ -2370,15 +2400,15 @@
         <v>412</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>6</v>
@@ -2393,12 +2423,12 @@
         <v>46</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>6</v>
@@ -2411,15 +2441,15 @@
         <v>185</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25" s="34" t="s">
         <v>6</v>
@@ -2431,15 +2461,15 @@
         <v>118</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>6</v>
@@ -2451,15 +2481,15 @@
         <v>50</v>
       </c>
       <c r="E26" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>7</v>
@@ -2471,15 +2501,15 @@
         <v>50</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>18</v>
@@ -2494,12 +2524,12 @@
         <v>46</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>8</v>
@@ -2511,15 +2541,15 @@
         <v>5</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B30" s="40" t="s">
         <v>8</v>
@@ -2534,12 +2564,12 @@
         <v>46</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B31" s="40" t="s">
         <v>8</v>
@@ -2551,15 +2581,15 @@
         <v>4</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="40" t="s">
         <v>8</v>
@@ -2571,15 +2601,15 @@
         <v>2</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>9</v>
@@ -2591,15 +2621,15 @@
         <v>1</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" s="42" t="s">
         <v>9</v>
@@ -2611,15 +2641,15 @@
         <v>1</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F34" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" s="44" t="s">
         <v>21</v>
@@ -2634,12 +2664,12 @@
         <v>46</v>
       </c>
       <c r="F35" s="45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>27</v>
@@ -2651,15 +2681,15 @@
         <v>0</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F36" s="47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>23</v>
@@ -2671,15 +2701,15 @@
         <v>46</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F37" s="49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B38" s="50" t="s">
         <v>22</v>
@@ -2691,15 +2721,15 @@
         <v>0</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F38" s="51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="52" t="s">
         <v>19</v>
@@ -2714,12 +2744,12 @@
         <v>46</v>
       </c>
       <c r="F39" s="53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B40" s="54" t="s">
         <v>20</v>
@@ -2734,12 +2764,12 @@
         <v>46</v>
       </c>
       <c r="F40" s="55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B41" s="56" t="s">
         <v>16</v>
@@ -2751,15 +2781,15 @@
         <v>1</v>
       </c>
       <c r="E41" s="57" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F41" s="57" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B42" s="58" t="s">
         <v>17</v>
@@ -2771,10 +2801,10 @@
         <v>1</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F42" s="59" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2800,10 +2830,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1">
@@ -3008,12 +3038,12 @@
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1">
       <c r="A27" s="60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
       <c r="A28" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28">
         <v>3215</v>
@@ -3041,16 +3071,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>71</v>
-      </c>
       <c r="D1" s="62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
@@ -3061,10 +3091,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -3075,10 +3105,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
@@ -3089,10 +3119,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
@@ -3106,7 +3136,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
@@ -3117,10 +3147,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
@@ -3131,10 +3161,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
@@ -3145,10 +3175,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
@@ -3162,7 +3192,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
@@ -3176,7 +3206,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
@@ -3187,10 +3217,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -3329,10 +3359,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
@@ -3367,10 +3397,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
delete added to all pages
</commit_message>
<xml_diff>
--- a/data/pool.xlsx
+++ b/data/pool.xlsx
@@ -891,7 +891,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <t>Courbis, Romeo:
 GSB battery whip w/öueller for universal battery fit</t>
@@ -2435,7 +2435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
@@ -2524,47 +2524,47 @@
         </is>
       </c>
       <c r="C3" s="81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="81" t="inlineStr">
         <is>
+          <t>UOulu</t>
+        </is>
+      </c>
+      <c r="F3" s="81" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="68">
+      <c r="A4" s="82" t="inlineStr">
+        <is>
+          <t>Geospace BN25 battery</t>
+        </is>
+      </c>
+      <c r="B4" s="82" t="inlineStr">
+        <is>
+          <t>BN25</t>
+        </is>
+      </c>
+      <c r="C4" s="83" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" s="83" t="n">
+        <v>25</v>
+      </c>
+      <c r="E4" s="83" t="inlineStr">
+        <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F3" s="81" t="inlineStr">
+      <c r="F4" s="83" t="inlineStr">
         <is>
           <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" s="68">
-      <c r="A4" s="80" t="inlineStr">
-        <is>
-          <t>Portable BMS (12 slots)</t>
-        </is>
-      </c>
-      <c r="B4" s="80" t="inlineStr">
-        <is>
-          <t>BMS12</t>
-        </is>
-      </c>
-      <c r="C4" s="81" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="81" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="81" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F4" s="81" t="inlineStr">
-        <is>
-          <t>Oulu</t>
         </is>
       </c>
     </row>
@@ -2580,10 +2580,10 @@
         </is>
       </c>
       <c r="C5" s="83" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D5" s="83" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E5" s="83" t="inlineStr">
         <is>
@@ -2597,142 +2597,142 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="68">
-      <c r="A6" s="82" t="inlineStr">
-        <is>
-          <t>Geospace BN25 battery</t>
-        </is>
-      </c>
-      <c r="B6" s="82" t="inlineStr">
-        <is>
-          <t>BN25</t>
-        </is>
-      </c>
-      <c r="C6" s="83" t="n">
-        <v>70</v>
-      </c>
-      <c r="D6" s="83" t="n">
-        <v>70</v>
-      </c>
-      <c r="E6" s="83" t="inlineStr">
+      <c r="A6" s="84" t="inlineStr">
+        <is>
+          <t>Geosapce BN32 battery</t>
+        </is>
+      </c>
+      <c r="B6" s="84" t="inlineStr">
+        <is>
+          <t>BN32</t>
+        </is>
+      </c>
+      <c r="C6" s="85" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" s="85" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" s="85" t="inlineStr">
+        <is>
+          <t>UOulu</t>
+        </is>
+      </c>
+      <c r="F6" s="85" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" s="68">
+      <c r="A7" s="88" t="inlineStr">
+        <is>
+          <t>GSB DC adapter</t>
+        </is>
+      </c>
+      <c r="B7" s="88" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C7" s="89" t="n">
+        <v>324</v>
+      </c>
+      <c r="D7" s="89" t="n">
+        <v>324</v>
+      </c>
+      <c r="E7" s="89" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F6" s="83" t="inlineStr">
+      <c r="F7" s="89" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" s="68">
-      <c r="A7" s="84" t="inlineStr">
-        <is>
-          <t>Geosapce BN32 battery</t>
-        </is>
-      </c>
-      <c r="B7" s="84" t="inlineStr">
-        <is>
-          <t>BN32</t>
-        </is>
-      </c>
-      <c r="C7" s="85" t="n">
-        <v>50</v>
-      </c>
-      <c r="D7" s="85" t="n">
-        <v>50</v>
-      </c>
-      <c r="E7" s="85" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F7" s="85" t="inlineStr">
-        <is>
-          <t>Oulu</t>
-        </is>
-      </c>
-    </row>
     <row r="8" ht="15.75" customHeight="1" s="68">
-      <c r="A8" s="86" t="inlineStr">
-        <is>
-          <t>Cable Minimus to 3ESPC</t>
-        </is>
-      </c>
-      <c r="B8" s="86" t="inlineStr">
-        <is>
-          <t>CABLEBB</t>
-        </is>
-      </c>
-      <c r="C8" s="87" t="n">
-        <v>46</v>
-      </c>
-      <c r="D8" s="87" t="n">
-        <v>46</v>
-      </c>
-      <c r="E8" s="87" t="inlineStr">
+      <c r="A8" s="92" t="inlineStr">
+        <is>
+          <t>GSB DTM (48 slots)</t>
+        </is>
+      </c>
+      <c r="B8" s="92" t="inlineStr">
+        <is>
+          <t>DTM48</t>
+        </is>
+      </c>
+      <c r="C8" s="93" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="93" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="93" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F8" s="87" t="inlineStr">
+      <c r="F8" s="93" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="68">
-      <c r="A9" s="88" t="inlineStr">
-        <is>
-          <t>GSB DC adapter</t>
-        </is>
-      </c>
-      <c r="B9" s="88" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="C9" s="89" t="n">
-        <v>324</v>
-      </c>
-      <c r="D9" s="89" t="n">
-        <v>324</v>
-      </c>
-      <c r="E9" s="89" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F9" s="89" t="inlineStr">
+      <c r="A9" s="92" t="inlineStr">
+        <is>
+          <t>GSB DTM (48 slots)</t>
+        </is>
+      </c>
+      <c r="B9" s="92" t="inlineStr">
+        <is>
+          <t>DTM48</t>
+        </is>
+      </c>
+      <c r="C9" s="93" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="93" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="93" t="inlineStr">
+        <is>
+          <t>GTK</t>
+        </is>
+      </c>
+      <c r="F9" s="93" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="68">
-      <c r="A10" s="90" t="inlineStr">
-        <is>
-          <t>GSB DTM (24 slots)</t>
-        </is>
-      </c>
-      <c r="B10" s="90" t="inlineStr">
-        <is>
-          <t>DTM24</t>
-        </is>
-      </c>
-      <c r="C10" s="91" t="n">
+      <c r="A10" s="92" t="inlineStr">
+        <is>
+          <t>GSB DTM (48 slots)</t>
+        </is>
+      </c>
+      <c r="B10" s="92" t="inlineStr">
+        <is>
+          <t>DTM48</t>
+        </is>
+      </c>
+      <c r="C10" s="93" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="91" t="n">
+      <c r="D10" s="93" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="91" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F10" s="91" t="inlineStr">
-        <is>
-          <t>Oulu</t>
+      <c r="E10" s="93" t="inlineStr">
+        <is>
+          <t>UTurku</t>
+        </is>
+      </c>
+      <c r="F10" s="93" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
         </is>
       </c>
     </row>
@@ -2748,185 +2748,187 @@
         </is>
       </c>
       <c r="C11" s="93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="93" t="inlineStr">
         <is>
+          <t>AaltoU</t>
+        </is>
+      </c>
+      <c r="F11" s="93" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="68">
+      <c r="A12" s="94" t="inlineStr">
+        <is>
+          <t>Fortis Accelerometer</t>
+        </is>
+      </c>
+      <c r="B12" s="94" t="inlineStr">
+        <is>
+          <t>FORTIS</t>
+        </is>
+      </c>
+      <c r="C12" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="95" t="inlineStr">
+        <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F11" s="93" t="inlineStr">
+      <c r="F12" s="95" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="68">
-      <c r="A12" s="92" t="inlineStr">
-        <is>
-          <t>GSB DTM (48 slots)</t>
-        </is>
-      </c>
-      <c r="B12" s="92" t="inlineStr">
-        <is>
-          <t>DTM48</t>
-        </is>
-      </c>
-      <c r="C12" s="93" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" s="93" t="n">
-        <v>3</v>
-      </c>
-      <c r="E12" s="93" t="inlineStr">
+    <row r="13" ht="15.75" customHeight="1" s="68">
+      <c r="A13" s="96" t="inlineStr">
+        <is>
+          <t>Battery GEL GF12063 Y04</t>
+        </is>
+      </c>
+      <c r="B13" s="96" t="inlineStr">
+        <is>
+          <t>GELBATTERY</t>
+        </is>
+      </c>
+      <c r="C13" s="97" t="n">
+        <v>20</v>
+      </c>
+      <c r="D13" s="97" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" s="97" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F13" s="97" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="68">
+      <c r="A14" s="98" t="inlineStr">
+        <is>
+          <t>GNSS antenna 10m</t>
+        </is>
+      </c>
+      <c r="B14" s="98" t="inlineStr">
+        <is>
+          <t>GNSS</t>
+        </is>
+      </c>
+      <c r="C14" s="99" t="n">
+        <v>46</v>
+      </c>
+      <c r="D14" s="99" t="n">
+        <v>46</v>
+      </c>
+      <c r="E14" s="99" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F14" s="99" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="68">
+      <c r="A15" s="100" t="inlineStr">
+        <is>
+          <t>GSB3 64GB</t>
+        </is>
+      </c>
+      <c r="B15" s="100" t="inlineStr">
+        <is>
+          <t>GSB3</t>
+        </is>
+      </c>
+      <c r="C15" s="101">
+        <f>261+151</f>
+        <v/>
+      </c>
+      <c r="D15" s="101" t="n">
+        <v>412</v>
+      </c>
+      <c r="E15" s="101" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F15" s="101" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" s="68">
+      <c r="A16" s="100" t="inlineStr">
+        <is>
+          <t>GSB3 64GB</t>
+        </is>
+      </c>
+      <c r="B16" s="100" t="inlineStr">
+        <is>
+          <t>GSB3</t>
+        </is>
+      </c>
+      <c r="C16" s="101" t="n">
+        <v>451</v>
+      </c>
+      <c r="D16" s="101" t="n">
+        <v>451</v>
+      </c>
+      <c r="E16" s="101" t="inlineStr">
         <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="F12" s="93" t="inlineStr">
+      <c r="F16" s="101" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" s="68">
-      <c r="A13" s="92" t="inlineStr">
-        <is>
-          <t>GSB DTM (48 slots)</t>
-        </is>
-      </c>
-      <c r="B13" s="92" t="inlineStr">
-        <is>
-          <t>DTM48</t>
-        </is>
-      </c>
-      <c r="C13" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="93" t="inlineStr">
+    <row r="17" ht="15.75" customHeight="1" s="68">
+      <c r="A17" s="100" t="inlineStr">
+        <is>
+          <t>GSB3 64GB</t>
+        </is>
+      </c>
+      <c r="B17" s="100" t="inlineStr">
+        <is>
+          <t>GSB3</t>
+        </is>
+      </c>
+      <c r="C17" s="101">
+        <f>147+38</f>
+        <v/>
+      </c>
+      <c r="D17" s="101" t="n">
+        <v>185</v>
+      </c>
+      <c r="E17" s="101" t="inlineStr">
         <is>
           <t>UTurku</t>
         </is>
       </c>
-      <c r="F13" s="93" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="68">
-      <c r="A14" s="92" t="inlineStr">
-        <is>
-          <t>GSB DTM (48 slots)</t>
-        </is>
-      </c>
-      <c r="B14" s="92" t="inlineStr">
-        <is>
-          <t>DTM48</t>
-        </is>
-      </c>
-      <c r="C14" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="93" t="inlineStr">
-        <is>
-          <t>AaltoU</t>
-        </is>
-      </c>
-      <c r="F14" s="93" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" s="68">
-      <c r="A15" s="94" t="inlineStr">
-        <is>
-          <t>Fortis Accelerometer</t>
-        </is>
-      </c>
-      <c r="B15" s="94" t="inlineStr">
-        <is>
-          <t>FORTIS</t>
-        </is>
-      </c>
-      <c r="C15" s="95" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="95" t="n">
-        <v>5</v>
-      </c>
-      <c r="E15" s="95" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F15" s="95" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1" s="68">
-      <c r="A16" s="96" t="inlineStr">
-        <is>
-          <t>Battery GEL GF12063 Y04</t>
-        </is>
-      </c>
-      <c r="B16" s="96" t="inlineStr">
-        <is>
-          <t>GELBATTERY</t>
-        </is>
-      </c>
-      <c r="C16" s="97" t="n">
-        <v>20</v>
-      </c>
-      <c r="D16" s="97" t="n">
-        <v>20</v>
-      </c>
-      <c r="E16" s="97" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F16" s="97" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1" s="68">
-      <c r="A17" s="98" t="inlineStr">
-        <is>
-          <t>GNSS antenna 10m</t>
-        </is>
-      </c>
-      <c r="B17" s="98" t="inlineStr">
-        <is>
-          <t>GNSS</t>
-        </is>
-      </c>
-      <c r="C17" s="99" t="n">
-        <v>46</v>
-      </c>
-      <c r="D17" s="99" t="n">
-        <v>46</v>
-      </c>
-      <c r="E17" s="99" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F17" s="99" t="inlineStr">
+      <c r="F17" s="101" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
@@ -2943,104 +2945,104 @@
           <t>GSB3</t>
         </is>
       </c>
-      <c r="C18" s="101">
+      <c r="C18" s="101" t="n">
+        <v>118</v>
+      </c>
+      <c r="D18" s="101" t="n">
+        <v>118</v>
+      </c>
+      <c r="E18" s="101" t="inlineStr">
+        <is>
+          <t>AaltoU</t>
+        </is>
+      </c>
+      <c r="F18" s="101" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="68">
+      <c r="A19" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE LF 5 Hz 3C</t>
+        </is>
+      </c>
+      <c r="B19" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE5HZ</t>
+        </is>
+      </c>
+      <c r="C19" s="103">
         <f>261+151</f>
         <v/>
       </c>
-      <c r="D18" s="101" t="n">
+      <c r="D19" s="103" t="n">
         <v>412</v>
       </c>
-      <c r="E18" s="101" t="inlineStr">
+      <c r="E19" s="103" t="inlineStr">
         <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F18" s="101" t="inlineStr">
+      <c r="F19" s="103" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1" s="68">
-      <c r="A19" s="100" t="inlineStr">
-        <is>
-          <t>GSB3 64GB</t>
-        </is>
-      </c>
-      <c r="B19" s="100" t="inlineStr">
-        <is>
-          <t>GSB3</t>
-        </is>
-      </c>
-      <c r="C19" s="101" t="n">
+    <row r="20" ht="15.75" customHeight="1" s="68">
+      <c r="A20" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE LF 5 Hz 3C</t>
+        </is>
+      </c>
+      <c r="B20" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE5HZ</t>
+        </is>
+      </c>
+      <c r="C20" s="103" t="n">
         <v>451</v>
       </c>
-      <c r="D19" s="101" t="n">
+      <c r="D20" s="103" t="n">
         <v>451</v>
       </c>
-      <c r="E19" s="101" t="inlineStr">
+      <c r="E20" s="103" t="inlineStr">
         <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="F19" s="101" t="inlineStr">
+      <c r="F20" s="103" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" s="68">
-      <c r="A20" s="100" t="inlineStr">
-        <is>
-          <t>GSB3 64GB</t>
-        </is>
-      </c>
-      <c r="B20" s="100" t="inlineStr">
-        <is>
-          <t>GSB3</t>
-        </is>
-      </c>
-      <c r="C20" s="101">
+    <row r="21" ht="15.75" customHeight="1" s="68">
+      <c r="A21" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE LF 5 Hz 3C</t>
+        </is>
+      </c>
+      <c r="B21" s="102" t="inlineStr">
+        <is>
+          <t>GS-ONE5HZ</t>
+        </is>
+      </c>
+      <c r="C21" s="103">
         <f>147+38</f>
         <v/>
       </c>
-      <c r="D20" s="101" t="n">
+      <c r="D21" s="103" t="n">
         <v>185</v>
       </c>
-      <c r="E20" s="101" t="inlineStr">
+      <c r="E21" s="103" t="inlineStr">
         <is>
           <t>UTurku</t>
         </is>
       </c>
-      <c r="F20" s="101" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" s="68">
-      <c r="A21" s="100" t="inlineStr">
-        <is>
-          <t>GSB3 64GB</t>
-        </is>
-      </c>
-      <c r="B21" s="100" t="inlineStr">
-        <is>
-          <t>GSB3</t>
-        </is>
-      </c>
-      <c r="C21" s="101" t="n">
-        <v>118</v>
-      </c>
-      <c r="D21" s="101" t="n">
-        <v>118</v>
-      </c>
-      <c r="E21" s="101" t="inlineStr">
-        <is>
-          <t>AaltoU</t>
-        </is>
-      </c>
-      <c r="F21" s="101" t="inlineStr">
+      <c r="F21" s="103" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
@@ -3057,16 +3059,15 @@
           <t>GS-ONE5HZ</t>
         </is>
       </c>
-      <c r="C22" s="103">
-        <f>261+151</f>
-        <v/>
+      <c r="C22" s="103" t="n">
+        <v>118</v>
       </c>
       <c r="D22" s="103" t="n">
-        <v>412</v>
+        <v>118</v>
       </c>
       <c r="E22" s="103" t="inlineStr">
         <is>
-          <t>UH</t>
+          <t>AaltoU</t>
         </is>
       </c>
       <c r="F22" s="103" t="inlineStr">
@@ -3087,160 +3088,159 @@
         </is>
       </c>
       <c r="C23" s="103" t="n">
-        <v>451</v>
+        <v>50</v>
       </c>
       <c r="D23" s="103" t="n">
-        <v>451</v>
+        <v>50</v>
       </c>
       <c r="E23" s="103" t="inlineStr">
         <is>
+          <t>UOulu</t>
+        </is>
+      </c>
+      <c r="F23" s="103" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" s="68">
+      <c r="A24" s="104" t="inlineStr">
+        <is>
+          <t>GSX3-LTE</t>
+        </is>
+      </c>
+      <c r="B24" s="104" t="inlineStr">
+        <is>
+          <t>GSX3</t>
+        </is>
+      </c>
+      <c r="C24" s="105" t="n">
+        <v>50</v>
+      </c>
+      <c r="D24" s="105" t="n">
+        <v>50</v>
+      </c>
+      <c r="E24" s="105" t="inlineStr">
+        <is>
+          <t>UOulu</t>
+        </is>
+      </c>
+      <c r="F24" s="105" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" s="68">
+      <c r="A25" s="106" t="inlineStr">
+        <is>
+          <t>SmartSolo IGU 16HR3C</t>
+        </is>
+      </c>
+      <c r="B25" s="106" t="inlineStr">
+        <is>
+          <t>IGU-16HR3C</t>
+        </is>
+      </c>
+      <c r="C25" s="107" t="n">
+        <v>71</v>
+      </c>
+      <c r="D25" s="107" t="n">
+        <v>71</v>
+      </c>
+      <c r="E25" s="107" t="inlineStr">
+        <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="F23" s="103" t="inlineStr">
+      <c r="F25" s="107" t="inlineStr">
+        <is>
+          <t>Espoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" s="68">
+      <c r="A26" s="108" t="inlineStr">
+        <is>
+          <t>GSB-LHR</t>
+        </is>
+      </c>
+      <c r="B26" s="108" t="inlineStr">
+        <is>
+          <t>LHR</t>
+        </is>
+      </c>
+      <c r="C26" s="109" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="109" t="n">
+        <v>5</v>
+      </c>
+      <c r="E26" s="109" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F26" s="109" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1" s="68">
-      <c r="A24" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE LF 5 Hz 3C</t>
-        </is>
-      </c>
-      <c r="B24" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="C24" s="103">
-        <f>147+38</f>
-        <v/>
-      </c>
-      <c r="D24" s="103" t="n">
-        <v>185</v>
-      </c>
-      <c r="E24" s="103" t="inlineStr">
+    <row r="27" ht="15.75" customHeight="1" s="68">
+      <c r="A27" s="108" t="inlineStr">
+        <is>
+          <t>GSB-LHR</t>
+        </is>
+      </c>
+      <c r="B27" s="108" t="inlineStr">
+        <is>
+          <t>LHR</t>
+        </is>
+      </c>
+      <c r="C27" s="109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="109" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="109" t="inlineStr">
+        <is>
+          <t>GTK</t>
+        </is>
+      </c>
+      <c r="F27" s="109" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" s="68">
+      <c r="A28" s="108" t="inlineStr">
+        <is>
+          <t>GSB-LHR</t>
+        </is>
+      </c>
+      <c r="B28" s="108" t="inlineStr">
+        <is>
+          <t>LHR</t>
+        </is>
+      </c>
+      <c r="C28" s="109" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="109" t="n">
+        <v>4</v>
+      </c>
+      <c r="E28" s="109" t="inlineStr">
         <is>
           <t>UTurku</t>
         </is>
       </c>
-      <c r="F24" s="103" t="inlineStr">
+      <c r="F28" s="109" t="inlineStr">
         <is>
           <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" s="68">
-      <c r="A25" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE LF 5 Hz 3C</t>
-        </is>
-      </c>
-      <c r="B25" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="C25" s="103" t="n">
-        <v>118</v>
-      </c>
-      <c r="D25" s="103" t="n">
-        <v>118</v>
-      </c>
-      <c r="E25" s="103" t="inlineStr">
-        <is>
-          <t>AaltoU</t>
-        </is>
-      </c>
-      <c r="F25" s="103" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" s="68">
-      <c r="A26" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE LF 5 Hz 3C</t>
-        </is>
-      </c>
-      <c r="B26" s="102" t="inlineStr">
-        <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="C26" s="103" t="n">
-        <v>50</v>
-      </c>
-      <c r="D26" s="103" t="n">
-        <v>50</v>
-      </c>
-      <c r="E26" s="103" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F26" s="103" t="inlineStr">
-        <is>
-          <t>Oulu</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1" s="68">
-      <c r="A27" s="104" t="inlineStr">
-        <is>
-          <t>GSX3-LTE</t>
-        </is>
-      </c>
-      <c r="B27" s="104" t="inlineStr">
-        <is>
-          <t>GSX3</t>
-        </is>
-      </c>
-      <c r="C27" s="105" t="n">
-        <v>50</v>
-      </c>
-      <c r="D27" s="105" t="n">
-        <v>50</v>
-      </c>
-      <c r="E27" s="105" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F27" s="105" t="inlineStr">
-        <is>
-          <t>Oulu</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" s="68">
-      <c r="A28" s="106" t="inlineStr">
-        <is>
-          <t>SmartSolo IGU 16HR3C</t>
-        </is>
-      </c>
-      <c r="B28" s="106" t="inlineStr">
-        <is>
-          <t>IGU-16HR3C</t>
-        </is>
-      </c>
-      <c r="C28" s="107" t="n">
-        <v>71</v>
-      </c>
-      <c r="D28" s="107" t="n">
-        <v>71</v>
-      </c>
-      <c r="E28" s="107" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="F28" s="107" t="inlineStr">
-        <is>
-          <t>Espoo</t>
         </is>
       </c>
     </row>
@@ -3256,386 +3256,305 @@
         </is>
       </c>
       <c r="C29" s="109" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D29" s="109" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E29" s="109" t="inlineStr">
         <is>
+          <t>UOulu</t>
+        </is>
+      </c>
+      <c r="F29" s="109" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1" s="68">
+      <c r="A30" s="110" t="inlineStr">
+        <is>
+          <t>GSB-LV</t>
+        </is>
+      </c>
+      <c r="B30" s="110" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="C30" s="111" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="111" t="inlineStr">
+        <is>
           <t>UH</t>
         </is>
       </c>
-      <c r="F29" s="109" t="inlineStr">
+      <c r="F30" s="111" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1" s="68">
-      <c r="A30" s="108" t="inlineStr">
-        <is>
-          <t>GSB-LHR</t>
-        </is>
-      </c>
-      <c r="B30" s="108" t="inlineStr">
-        <is>
-          <t>LHR</t>
-        </is>
-      </c>
-      <c r="C30" s="109" t="n">
+    <row r="31" ht="15.75" customHeight="1" s="68">
+      <c r="A31" s="110" t="inlineStr">
+        <is>
+          <t>GSB-LV</t>
+        </is>
+      </c>
+      <c r="B31" s="110" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="C31" s="111" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="109" t="n">
+      <c r="D31" s="111" t="n">
         <v>1</v>
       </c>
-      <c r="E30" s="109" t="inlineStr">
+      <c r="E31" s="111" t="inlineStr">
+        <is>
+          <t>AaltoU</t>
+        </is>
+      </c>
+      <c r="F31" s="111" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1" s="68">
+      <c r="A32" s="112" t="inlineStr">
+        <is>
+          <t>SmartSolo magnet</t>
+        </is>
+      </c>
+      <c r="B32" s="112" t="inlineStr">
+        <is>
+          <t>MAGNET</t>
+        </is>
+      </c>
+      <c r="C32" s="113" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" s="113" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" s="113" t="inlineStr">
         <is>
           <t>GTK</t>
         </is>
       </c>
-      <c r="F30" s="109" t="inlineStr">
+      <c r="F32" s="113" t="inlineStr">
+        <is>
+          <t>Espoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" s="68">
+      <c r="A33" s="114" t="inlineStr">
+        <is>
+          <t>Mascot battery charger</t>
+        </is>
+      </c>
+      <c r="B33" s="114" t="inlineStr">
+        <is>
+          <t>MASCOT</t>
+        </is>
+      </c>
+      <c r="C33" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="115" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F33" s="115" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1" s="68">
-      <c r="A31" s="108" t="inlineStr">
-        <is>
-          <t>GSB-LHR</t>
-        </is>
-      </c>
-      <c r="B31" s="108" t="inlineStr">
-        <is>
-          <t>LHR</t>
-        </is>
-      </c>
-      <c r="C31" s="109" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" s="109" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" s="109" t="inlineStr">
-        <is>
-          <t>UTurku</t>
-        </is>
-      </c>
-      <c r="F31" s="109" t="inlineStr">
+    <row r="34" ht="15.75" customHeight="1" s="68">
+      <c r="A34" s="116" t="inlineStr">
+        <is>
+          <t>Güralp Minimus digitizer</t>
+        </is>
+      </c>
+      <c r="B34" s="116" t="inlineStr">
+        <is>
+          <t>MINIMUS</t>
+        </is>
+      </c>
+      <c r="C34" s="117" t="n">
+        <v>46</v>
+      </c>
+      <c r="D34" s="117" t="n">
+        <v>46</v>
+      </c>
+      <c r="E34" s="117" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F34" s="117" t="inlineStr">
         <is>
           <t>Helsinki</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1" s="68">
-      <c r="A32" s="108" t="inlineStr">
-        <is>
-          <t>GSB-LHR</t>
-        </is>
-      </c>
-      <c r="B32" s="108" t="inlineStr">
-        <is>
-          <t>LHR</t>
-        </is>
-      </c>
-      <c r="C32" s="109" t="n">
+    <row r="35" ht="15.75" customHeight="1" s="68">
+      <c r="A35" s="118" t="inlineStr">
+        <is>
+          <t>Source Decoder Recorder</t>
+        </is>
+      </c>
+      <c r="B35" s="118" t="inlineStr">
+        <is>
+          <t>SDRX</t>
+        </is>
+      </c>
+      <c r="C35" s="119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="119" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="F35" s="119" t="inlineStr">
+        <is>
+          <t>Helsinki</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="68">
+      <c r="A36" s="120" t="inlineStr">
+        <is>
+          <t>SmartSolo Battery charger</t>
+        </is>
+      </c>
+      <c r="B36" s="120" t="inlineStr">
+        <is>
+          <t>SmartsoloCharger</t>
+        </is>
+      </c>
+      <c r="C36" s="121" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="121" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="121" t="inlineStr">
+        <is>
+          <t>GTK</t>
+        </is>
+      </c>
+      <c r="F36" s="121" t="inlineStr">
+        <is>
+          <t>Espoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="68">
+      <c r="A37" s="122" t="inlineStr">
+        <is>
+          <t>SmartSolo Data Rack</t>
+        </is>
+      </c>
+      <c r="B37" s="122" t="inlineStr">
+        <is>
+          <t>SmartsoloRack</t>
+        </is>
+      </c>
+      <c r="C37" s="123" t="n">
         <v>2</v>
       </c>
-      <c r="D32" s="109" t="n">
+      <c r="D37" s="123" t="n">
         <v>2</v>
       </c>
-      <c r="E32" s="109" t="inlineStr">
+      <c r="E37" s="123" t="inlineStr">
+        <is>
+          <t>GTK</t>
+        </is>
+      </c>
+      <c r="F37" s="123" t="inlineStr">
+        <is>
+          <t>Espoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" s="68">
+      <c r="A38" s="124" t="inlineStr">
+        <is>
+          <t>Panasonic FZ-55 toughbook</t>
+        </is>
+      </c>
+      <c r="B38" s="124" t="inlineStr">
+        <is>
+          <t>TOUGHBOOK</t>
+        </is>
+      </c>
+      <c r="C38" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="125" t="inlineStr">
         <is>
           <t>UOulu</t>
         </is>
       </c>
-      <c r="F32" s="109" t="inlineStr">
+      <c r="F38" s="125" t="inlineStr">
         <is>
           <t>Oulu</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1" s="68">
-      <c r="A33" s="110" t="inlineStr">
-        <is>
-          <t>GSB-LV</t>
-        </is>
-      </c>
-      <c r="B33" s="110" t="inlineStr">
-        <is>
-          <t>LV</t>
-        </is>
-      </c>
-      <c r="C33" s="111" t="n">
+    <row r="39" ht="15.75" customHeight="1" s="68">
+      <c r="A39" s="126" t="inlineStr">
+        <is>
+          <t>Zbook Fury</t>
+        </is>
+      </c>
+      <c r="B39" s="126" t="inlineStr">
+        <is>
+          <t>ZBOOK</t>
+        </is>
+      </c>
+      <c r="C39" s="127" t="n">
         <v>1</v>
       </c>
-      <c r="D33" s="111" t="n">
+      <c r="D39" s="127" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="111" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F33" s="111" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1" s="68">
-      <c r="A34" s="110" t="inlineStr">
-        <is>
-          <t>GSB-LV</t>
-        </is>
-      </c>
-      <c r="B34" s="110" t="inlineStr">
-        <is>
-          <t>LV</t>
-        </is>
-      </c>
-      <c r="C34" s="111" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="111" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="111" t="inlineStr">
-        <is>
-          <t>AaltoU</t>
-        </is>
-      </c>
-      <c r="F34" s="111" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1" s="68">
-      <c r="A35" s="112" t="inlineStr">
-        <is>
-          <t>SmartSolo magnet</t>
-        </is>
-      </c>
-      <c r="B35" s="112" t="inlineStr">
-        <is>
-          <t>MAGNET</t>
-        </is>
-      </c>
-      <c r="C35" s="113" t="n">
-        <v>4</v>
-      </c>
-      <c r="D35" s="113" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="113" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="F35" s="113" t="inlineStr">
-        <is>
-          <t>Espoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" s="68">
-      <c r="A36" s="114" t="inlineStr">
-        <is>
-          <t>Mascot battery charger</t>
-        </is>
-      </c>
-      <c r="B36" s="114" t="inlineStr">
-        <is>
-          <t>MASCOT</t>
-        </is>
-      </c>
-      <c r="C36" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="115" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F36" s="115" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" s="68">
-      <c r="A37" s="116" t="inlineStr">
-        <is>
-          <t>Güralp Minimus digitizer</t>
-        </is>
-      </c>
-      <c r="B37" s="116" t="inlineStr">
-        <is>
-          <t>MINIMUS</t>
-        </is>
-      </c>
-      <c r="C37" s="117" t="n">
-        <v>46</v>
-      </c>
-      <c r="D37" s="117" t="n">
-        <v>46</v>
-      </c>
-      <c r="E37" s="117" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F37" s="117" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1" s="68">
-      <c r="A38" s="118" t="inlineStr">
-        <is>
-          <t>Source Decoder Recorder</t>
-        </is>
-      </c>
-      <c r="B38" s="118" t="inlineStr">
-        <is>
-          <t>SDRX</t>
-        </is>
-      </c>
-      <c r="C38" s="119" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="119" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="119" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="F38" s="119" t="inlineStr">
-        <is>
-          <t>Helsinki</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1" s="68">
-      <c r="A39" s="120" t="inlineStr">
-        <is>
-          <t>SmartSolo Battery charger</t>
-        </is>
-      </c>
-      <c r="B39" s="120" t="inlineStr">
-        <is>
-          <t>SmartsoloCharger</t>
-        </is>
-      </c>
-      <c r="C39" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="D39" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="121" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="F39" s="121" t="inlineStr">
-        <is>
-          <t>Espoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1" s="68">
-      <c r="A40" s="122" t="inlineStr">
-        <is>
-          <t>SmartSolo Data Rack</t>
-        </is>
-      </c>
-      <c r="B40" s="122" t="inlineStr">
-        <is>
-          <t>SmartsoloRack</t>
-        </is>
-      </c>
-      <c r="C40" s="123" t="n">
-        <v>2</v>
-      </c>
-      <c r="D40" s="123" t="n">
-        <v>2</v>
-      </c>
-      <c r="E40" s="123" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="F40" s="123" t="inlineStr">
-        <is>
-          <t>Espoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1" s="68">
-      <c r="A41" s="124" t="inlineStr">
-        <is>
-          <t>Panasonic FZ-55 toughbook</t>
-        </is>
-      </c>
-      <c r="B41" s="124" t="inlineStr">
-        <is>
-          <t>TOUGHBOOK</t>
-        </is>
-      </c>
-      <c r="C41" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="125" t="inlineStr">
+      <c r="E39" s="127" t="inlineStr">
         <is>
           <t>UOulu</t>
         </is>
       </c>
-      <c r="F41" s="125" t="inlineStr">
+      <c r="F39" s="127" t="inlineStr">
         <is>
           <t>Oulu</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1" s="68">
-      <c r="A42" s="126" t="inlineStr">
-        <is>
-          <t>Zbook Fury</t>
-        </is>
-      </c>
-      <c r="B42" s="126" t="inlineStr">
-        <is>
-          <t>ZBOOK</t>
-        </is>
-      </c>
-      <c r="C42" s="127" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="127" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="127" t="inlineStr">
-        <is>
-          <t>UOulu</t>
-        </is>
-      </c>
-      <c r="F42" s="127" t="inlineStr">
-        <is>
-          <t>Oulu</t>
-        </is>
-      </c>
-    </row>
+    <row r="40" ht="15.75" customHeight="1" s="68"/>
+    <row r="41" ht="15.75" customHeight="1" s="68"/>
+    <row r="42" ht="15.75" customHeight="1" s="68"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3954,7 +3873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3996,7 +3915,7 @@
         </is>
       </c>
       <c r="B2" s="67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="67" t="inlineStr">
         <is>
@@ -4005,10 +3924,14 @@
       </c>
       <c r="D2" s="67" t="inlineStr">
         <is>
-          <t>Broken</t>
-        </is>
-      </c>
-      <c r="E2" s="67" t="inlineStr"/>
+          <t>Lost</t>
+        </is>
+      </c>
+      <c r="E2" s="67" t="inlineStr">
+        <is>
+          <t>it was all broken</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="67" t="inlineStr">
@@ -4017,23 +3940,19 @@
         </is>
       </c>
       <c r="B3" s="67" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3" s="67" t="inlineStr">
         <is>
-          <t>UH</t>
+          <t>GTK</t>
         </is>
       </c>
       <c r="D3" s="67" t="inlineStr">
         <is>
-          <t>Lost</t>
-        </is>
-      </c>
-      <c r="E3" s="67" t="inlineStr">
-        <is>
-          <t>it was all broken</t>
-        </is>
-      </c>
+          <t>Broken</t>
+        </is>
+      </c>
+      <c r="E3" s="67" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="67" t="inlineStr">
@@ -4042,16 +3961,16 @@
         </is>
       </c>
       <c r="B4" s="67" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C4" s="67" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Aalto</t>
         </is>
       </c>
       <c r="D4" s="67" t="inlineStr">
         <is>
-          <t>Collapsed</t>
+          <t>Broken</t>
         </is>
       </c>
       <c r="E4" s="67" t="inlineStr"/>
@@ -4059,11 +3978,11 @@
     <row r="5">
       <c r="A5" s="67" t="inlineStr">
         <is>
-          <t>GSB3</t>
+          <t>GS-ONE5HZ</t>
         </is>
       </c>
       <c r="B5" s="67" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="67" t="inlineStr">
         <is>
@@ -4080,11 +3999,11 @@
     <row r="6">
       <c r="A6" s="67" t="inlineStr">
         <is>
-          <t>GSB3</t>
+          <t>GS-ONE5HZ</t>
         </is>
       </c>
       <c r="B6" s="67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="67" t="inlineStr">
         <is>
@@ -4101,163 +4020,111 @@
     <row r="7">
       <c r="A7" s="67" t="inlineStr">
         <is>
-          <t>GSB3</t>
+          <t>LHR</t>
         </is>
       </c>
       <c r="B7" s="67" t="n">
-        <v>1</v>
+        <v>444</v>
       </c>
       <c r="C7" s="67" t="inlineStr">
         <is>
-          <t>Aalto</t>
+          <t>445</t>
         </is>
       </c>
       <c r="D7" s="67" t="inlineStr">
         <is>
-          <t>Broken</t>
-        </is>
-      </c>
-      <c r="E7" s="67" t="inlineStr"/>
+          <t>446</t>
+        </is>
+      </c>
+      <c r="E7" s="67" t="inlineStr">
+        <is>
+          <t>447 des</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="67" t="inlineStr">
         <is>
-          <t>GS-ONE5HZ</t>
+          <t>LV</t>
         </is>
       </c>
       <c r="B8" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="67" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="D8" s="67" t="inlineStr">
-        <is>
-          <t>Lost</t>
-        </is>
-      </c>
-      <c r="E8" s="67" t="inlineStr"/>
+        <v>654</v>
+      </c>
+      <c r="C8" s="67" t="n"/>
+      <c r="D8" s="67" t="n"/>
+      <c r="E8" s="67" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="67" t="inlineStr">
         <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="B9" s="67" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" s="67" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="D9" s="67" t="inlineStr">
-        <is>
-          <t>Broken</t>
-        </is>
-      </c>
+          <t>BN25</t>
+        </is>
+      </c>
+      <c r="B9" s="67" t="inlineStr"/>
+      <c r="C9" s="67" t="inlineStr"/>
+      <c r="D9" s="67" t="inlineStr"/>
       <c r="E9" s="67" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="67" t="inlineStr">
         <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="B10" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="67" t="inlineStr">
-        <is>
-          <t>GTK</t>
-        </is>
-      </c>
-      <c r="D10" s="67" t="inlineStr">
-        <is>
-          <t>Lost</t>
-        </is>
-      </c>
+          <t>BN32</t>
+        </is>
+      </c>
+      <c r="B10" s="67" t="inlineStr"/>
+      <c r="C10" s="67" t="inlineStr"/>
+      <c r="D10" s="67" t="inlineStr"/>
       <c r="E10" s="67" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="67" t="inlineStr">
         <is>
-          <t>GS-ONE5HZ</t>
-        </is>
-      </c>
-      <c r="B11" s="67" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="67" t="inlineStr">
-        <is>
-          <t>Turku</t>
-        </is>
-      </c>
-      <c r="D11" s="67" t="inlineStr">
-        <is>
-          <t>Broken</t>
-        </is>
-      </c>
+          <t>DTM48</t>
+        </is>
+      </c>
+      <c r="B11" s="67" t="inlineStr"/>
+      <c r="C11" s="67" t="inlineStr"/>
+      <c r="D11" s="67" t="inlineStr"/>
       <c r="E11" s="67" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="67" t="inlineStr">
         <is>
-          <t>GSX3</t>
-        </is>
-      </c>
-      <c r="B12" s="67" t="n">
-        <v>34</v>
-      </c>
-      <c r="C12" s="67" t="n"/>
-      <c r="D12" s="67" t="n"/>
-      <c r="E12" s="67" t="n"/>
+          <t>DTM24</t>
+        </is>
+      </c>
+      <c r="B12" s="67" t="inlineStr"/>
+      <c r="C12" s="67" t="inlineStr"/>
+      <c r="D12" s="67" t="inlineStr"/>
+      <c r="E12" s="67" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="67" t="inlineStr">
         <is>
-          <t>LHR</t>
-        </is>
-      </c>
-      <c r="B13" s="67" t="n">
-        <v>444</v>
-      </c>
-      <c r="C13" s="67" t="inlineStr">
-        <is>
-          <t>445</t>
-        </is>
-      </c>
-      <c r="D13" s="67" t="inlineStr">
-        <is>
-          <t>446</t>
-        </is>
-      </c>
-      <c r="E13" s="67" t="inlineStr">
-        <is>
-          <t>447 des</t>
-        </is>
-      </c>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="B13" s="67" t="inlineStr"/>
+      <c r="C13" s="67" t="inlineStr"/>
+      <c r="D13" s="67" t="inlineStr"/>
+      <c r="E13" s="67" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="67" t="inlineStr">
         <is>
-          <t>LV</t>
-        </is>
-      </c>
-      <c r="B14" s="67" t="n">
-        <v>654</v>
-      </c>
-      <c r="C14" s="67" t="n"/>
-      <c r="D14" s="67" t="n"/>
-      <c r="E14" s="67" t="n"/>
+          <t>BMS12</t>
+        </is>
+      </c>
+      <c r="B14" s="67" t="inlineStr"/>
+      <c r="C14" s="67" t="inlineStr"/>
+      <c r="D14" s="67" t="inlineStr"/>
+      <c r="E14" s="67" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="67" t="inlineStr">
         <is>
-          <t>BN25</t>
+          <t>TOUGHBOOK</t>
         </is>
       </c>
       <c r="B15" s="67" t="inlineStr"/>
@@ -4268,7 +4135,7 @@
     <row r="16">
       <c r="A16" s="67" t="inlineStr">
         <is>
-          <t>BN32</t>
+          <t>ZBOOK</t>
         </is>
       </c>
       <c r="B16" s="67" t="inlineStr"/>
@@ -4279,7 +4146,7 @@
     <row r="17">
       <c r="A17" s="67" t="inlineStr">
         <is>
-          <t>DTM48</t>
+          <t>IGU-16HR3C</t>
         </is>
       </c>
       <c r="B17" s="67" t="inlineStr"/>
@@ -4290,7 +4157,7 @@
     <row r="18">
       <c r="A18" s="67" t="inlineStr">
         <is>
-          <t>DTM24</t>
+          <t>SmartsoloCharger</t>
         </is>
       </c>
       <c r="B18" s="67" t="inlineStr"/>
@@ -4301,7 +4168,7 @@
     <row r="19">
       <c r="A19" s="67" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>SmartsoloRack</t>
         </is>
       </c>
       <c r="B19" s="67" t="inlineStr"/>
@@ -4312,7 +4179,7 @@
     <row r="20">
       <c r="A20" s="67" t="inlineStr">
         <is>
-          <t>BMS12</t>
+          <t>MAGNET</t>
         </is>
       </c>
       <c r="B20" s="67" t="inlineStr"/>
@@ -4323,7 +4190,7 @@
     <row r="21">
       <c r="A21" s="67" t="inlineStr">
         <is>
-          <t>TOUGHBOOK</t>
+          <t>SDRX</t>
         </is>
       </c>
       <c r="B21" s="67" t="inlineStr"/>
@@ -4334,18 +4201,28 @@
     <row r="22">
       <c r="A22" s="67" t="inlineStr">
         <is>
-          <t>ZBOOK</t>
-        </is>
-      </c>
-      <c r="B22" s="67" t="inlineStr"/>
-      <c r="C22" s="67" t="inlineStr"/>
-      <c r="D22" s="67" t="inlineStr"/>
+          <t>MINIMUS</t>
+        </is>
+      </c>
+      <c r="B22" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="67" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="D22" s="67" t="inlineStr">
+        <is>
+          <t>Broken</t>
+        </is>
+      </c>
       <c r="E22" s="67" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="67" t="inlineStr">
         <is>
-          <t>IGU-16HR3C</t>
+          <t>3ESPC</t>
         </is>
       </c>
       <c r="B23" s="67" t="inlineStr"/>
@@ -4356,7 +4233,7 @@
     <row r="24">
       <c r="A24" s="67" t="inlineStr">
         <is>
-          <t>SmartsoloCharger</t>
+          <t>GNSS</t>
         </is>
       </c>
       <c r="B24" s="67" t="inlineStr"/>
@@ -4367,7 +4244,7 @@
     <row r="25">
       <c r="A25" s="67" t="inlineStr">
         <is>
-          <t>SmartsoloRack</t>
+          <t>CABLEBB</t>
         </is>
       </c>
       <c r="B25" s="67" t="inlineStr"/>
@@ -4378,18 +4255,28 @@
     <row r="26">
       <c r="A26" s="67" t="inlineStr">
         <is>
-          <t>MAGNET</t>
-        </is>
-      </c>
-      <c r="B26" s="67" t="inlineStr"/>
-      <c r="C26" s="67" t="inlineStr"/>
-      <c r="D26" s="67" t="inlineStr"/>
+          <t>MASCOT</t>
+        </is>
+      </c>
+      <c r="B26" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="67" t="inlineStr">
+        <is>
+          <t>UH</t>
+        </is>
+      </c>
+      <c r="D26" s="67" t="inlineStr">
+        <is>
+          <t>Broken</t>
+        </is>
+      </c>
       <c r="E26" s="67" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="67" t="inlineStr">
         <is>
-          <t>SDRX</t>
+          <t>GELBATTERY</t>
         </is>
       </c>
       <c r="B27" s="67" t="inlineStr"/>
@@ -4400,199 +4287,113 @@
     <row r="28">
       <c r="A28" s="67" t="inlineStr">
         <is>
-          <t>MINIMUS</t>
-        </is>
-      </c>
-      <c r="B28" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="67" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="D28" s="67" t="inlineStr">
-        <is>
-          <t>Broken</t>
-        </is>
-      </c>
+          <t>FORTIS</t>
+        </is>
+      </c>
+      <c r="B28" s="67" t="inlineStr"/>
+      <c r="C28" s="67" t="inlineStr"/>
+      <c r="D28" s="67" t="inlineStr"/>
       <c r="E28" s="67" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="67" t="inlineStr">
-        <is>
-          <t>3ESPC</t>
-        </is>
-      </c>
-      <c r="B29" s="67" t="inlineStr"/>
+      <c r="A29" s="67" t="inlineStr"/>
+      <c r="B29" s="67" t="n">
+        <v>0</v>
+      </c>
       <c r="C29" s="67" t="inlineStr"/>
       <c r="D29" s="67" t="inlineStr"/>
       <c r="E29" s="67" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="67" t="inlineStr">
-        <is>
-          <t>GNSS</t>
-        </is>
-      </c>
-      <c r="B30" s="67" t="inlineStr"/>
+      <c r="A30" s="67" t="inlineStr"/>
+      <c r="B30" s="67" t="n">
+        <v>0</v>
+      </c>
       <c r="C30" s="67" t="inlineStr"/>
       <c r="D30" s="67" t="inlineStr"/>
       <c r="E30" s="67" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="67" t="inlineStr">
-        <is>
-          <t>CABLEBB</t>
-        </is>
-      </c>
-      <c r="B31" s="67" t="inlineStr"/>
+      <c r="A31" s="67" t="inlineStr"/>
+      <c r="B31" s="67" t="n">
+        <v>0</v>
+      </c>
       <c r="C31" s="67" t="inlineStr"/>
       <c r="D31" s="67" t="inlineStr"/>
       <c r="E31" s="67" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="67" t="inlineStr">
-        <is>
-          <t>MASCOT</t>
-        </is>
-      </c>
+      <c r="A32" s="67" t="inlineStr"/>
       <c r="B32" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="67" t="inlineStr">
-        <is>
-          <t>UH</t>
-        </is>
-      </c>
-      <c r="D32" s="67" t="inlineStr">
-        <is>
-          <t>Broken</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C32" s="67" t="inlineStr"/>
+      <c r="D32" s="67" t="inlineStr"/>
       <c r="E32" s="67" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="67" t="inlineStr">
-        <is>
-          <t>GELBATTERY</t>
-        </is>
-      </c>
-      <c r="B33" s="67" t="inlineStr"/>
+      <c r="A33" s="67" t="inlineStr"/>
+      <c r="B33" s="67" t="n">
+        <v>0</v>
+      </c>
       <c r="C33" s="67" t="inlineStr"/>
       <c r="D33" s="67" t="inlineStr"/>
       <c r="E33" s="67" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" s="67" t="inlineStr">
-        <is>
-          <t>FORTIS</t>
-        </is>
-      </c>
-      <c r="B34" s="67" t="inlineStr"/>
+      <c r="A34" s="67" t="inlineStr"/>
+      <c r="B34" s="67" t="n">
+        <v>0</v>
+      </c>
       <c r="C34" s="67" t="inlineStr"/>
       <c r="D34" s="67" t="inlineStr"/>
       <c r="E34" s="67" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" s="67" t="inlineStr"/>
+      <c r="A35" s="67" t="inlineStr">
+        <is>
+          <t>BMS12</t>
+        </is>
+      </c>
       <c r="B35" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" s="67" t="inlineStr"/>
-      <c r="D35" s="67" t="inlineStr"/>
-      <c r="E35" s="67" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="C35" s="67" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D35" s="67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E35" s="67" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="67" t="inlineStr"/>
+      <c r="A36" s="67" t="inlineStr">
+        <is>
+          <t>BN25</t>
+        </is>
+      </c>
       <c r="B36" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="67" t="inlineStr"/>
-      <c r="D36" s="67" t="inlineStr"/>
-      <c r="E36" s="67" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="67" t="inlineStr"/>
-      <c r="B37" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" s="67" t="inlineStr"/>
-      <c r="D37" s="67" t="inlineStr"/>
-      <c r="E37" s="67" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="67" t="inlineStr"/>
-      <c r="B38" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" s="67" t="inlineStr"/>
-      <c r="D38" s="67" t="inlineStr"/>
-      <c r="E38" s="67" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="67" t="inlineStr"/>
-      <c r="B39" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="67" t="inlineStr"/>
-      <c r="D39" s="67" t="inlineStr"/>
-      <c r="E39" s="67" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="67" t="inlineStr"/>
-      <c r="B40" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="67" t="inlineStr"/>
-      <c r="D40" s="67" t="inlineStr"/>
-      <c r="E40" s="67" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="67" t="inlineStr">
-        <is>
-          <t>BMS12</t>
-        </is>
-      </c>
-      <c r="B41" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="67" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D41" s="67" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E41" s="67" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="67" t="inlineStr">
-        <is>
-          <t>BN25</t>
-        </is>
-      </c>
-      <c r="B42" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="C42" s="67" t="inlineStr">
+      <c r="C36" s="67" t="inlineStr">
         <is>
           <t>12ww</t>
         </is>
       </c>
-      <c r="D42" s="67" t="inlineStr">
+      <c r="D36" s="67" t="inlineStr">
         <is>
           <t>13ww</t>
         </is>
       </c>
-      <c r="E42" s="67" t="inlineStr">
+      <c r="E36" s="67" t="inlineStr">
         <is>
           <t>14ww</t>
         </is>

</xml_diff>